<commit_message>
Update the reading list analysis.
</commit_message>
<xml_diff>
--- a/ReadingListAnalysis.xlsx
+++ b/ReadingListAnalysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usachcl-my.sharepoint.com/personal/luis_rojo_g_usach_cl/Documents/PhD/Literature_Review/Coordinated-Charging-Literature-Review/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3851" documentId="8_{11581BE0-299A-8F49-932A-90BA12D1B0CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4FFC7CB0-807A-5344-B3E5-2C55717E35E1}"/>
+  <xr:revisionPtr revIDLastSave="4057" documentId="8_{11581BE0-299A-8F49-932A-90BA12D1B0CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DA67CEA2-C476-8943-BB87-41D749E69898}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -678,7 +678,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2074" uniqueCount="958">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2262" uniqueCount="987">
   <si>
     <t>Title</t>
   </si>
@@ -3220,9 +3220,6 @@
   </si>
   <si>
     <t>Games; Urban areas; Pricing; Charging stations; Vehicles; Employment; Standards; Electric vehicles; trilevel optimization; smart charging; coupled transportation-electrical systems</t>
-  </si>
-  <si>
-    <t>Given</t>
   </si>
   <si>
     <t>CSO</t>
@@ -3571,6 +3568,121 @@
   </si>
   <si>
     <t>Section 2 and 8 are useful</t>
+  </si>
+  <si>
+    <t>PV</t>
+  </si>
+  <si>
+    <t>@article{zhao2017real,
+  title={Real-time optimal energy and reserve management of electric vehicle fast charging station: Hierarchical game approach},
+  author={Zhao, Tianyang and Li, Yuanzheng and Pan, Xuewei and Wang, Peng and Zhang, Jianhua},
+  journal={IEEE Transactions on Smart Grid},
+  volume={9},
+  number={5},
+  pages={5357--5370},
+  year={2017},
+  publisher={IEEE}
+}</t>
+  </si>
+  <si>
+    <t>Fast charging station, regulation reserve, game theory, bi-level optimization</t>
+  </si>
+  <si>
+    <t>Real-time</t>
+  </si>
+  <si>
+    <t>5 min</t>
+  </si>
+  <si>
+    <t>Decentralized</t>
+  </si>
+  <si>
+    <t>Homogeneous (120 kW)</t>
+  </si>
+  <si>
+    <t>It handles a single charging facility</t>
+  </si>
+  <si>
+    <t>FIFO</t>
+  </si>
+  <si>
+    <t>Station</t>
+  </si>
+  <si>
+    <t>This work proposes a decentralized bi-level optimization model that handles different Evs that require a minimum amount of charge. However, the charging schedule (or plan as called in the article) does not change over time, i.e., once is constructed it holds until the SoC lies within a desired interval. The charging process considers a V2G flow such that each player maximize their profits with the use of a BESS and a PV power generation.</t>
+  </si>
+  <si>
+    <t>Although this seems to be one of the first studies that use the idea of V2G, it turns out to be difficult for the reader to understand how the charging/discharging process works from the indexing of the variables, and the fact that the charging coordination is decided at the beginning and not throughout time. Besides, the idea of not considering arrival and departure time is far from a real scenario when a public charging station is being analyzed. Finally, not to consider the charging pile dispatching and only power flows may not provide accurate results in presence of short dwell times and low PV power generation.</t>
+  </si>
+  <si>
+    <t>Energy management system, electric vehicle, electric vehicle charging station, tri-level game theory</t>
+  </si>
+  <si>
+    <t>It uses a IEEE 9-bus system</t>
+  </si>
+  <si>
+    <t>@article{shakerighadi2018hierarchical,
+  title={A hierarchical game theoretical approach for energy management of electric vehicles and charging stations in smart grids},
+  author={Shakerighadi, Bahram and Anvari-Moghaddam, Amjad and Ebrahimzadeh, Esmaeil and Blaabjerg, Frede and Bak, Claus Leth},
+  journal={Ieee Access},
+  volume={6},
+  pages={67223--67234},
+  year={2018},
+  publisher={IEEE}
+}</t>
+  </si>
+  <si>
+    <t>Heterogeneous</t>
+  </si>
+  <si>
+    <t>Constant</t>
+  </si>
+  <si>
+    <t>This work proposes a decentralized tri-level model that aims to coordinate the charging considering bus voltage constraint on price-based incentives. To this end, the energy price is determined by the charging load ocurring at the charging station considering that EVs may select the CS where to charge. The model is solved via backward induction upon a bottom-up schema.</t>
+  </si>
+  <si>
+    <t>A decentralized control allows the inclusion of several EVs' characteristics; however, none of them is taken into account. Not even the minimum requested charging. Besides, the charging schedule is fixed and does not change throughout time. Although this may not be a constraint if the model is solved at each time slot, there is no details about it.</t>
+  </si>
+  <si>
+    <t>It is not well written</t>
+  </si>
+  <si>
+    <t>This is interesting for challenges, but it is not the coordination study I am looking for</t>
+  </si>
+  <si>
+    <t>@article{subramanian2019two,
+  title={A two-layer model for dynamic pricing of electricity and optimal charging of electric vehicles under price spikes},
+  author={Subramanian, Vignesh and Das, Tapas K},
+  journal={Energy},
+  volume={167},
+  pages={1266--1277},
+  year={2019},
+  publisher={Elsevier}
+}</t>
+  </si>
+  <si>
+    <t>Dynamic pricing, electric vehicles, demand response, mathematical program with equilibrium constraints, robust optimization</t>
+  </si>
+  <si>
+    <t>Bus</t>
+  </si>
+  <si>
+    <t>Heterogenous</t>
+  </si>
+  <si>
+    <t>Homogeneous (11.5 kW)</t>
+  </si>
+  <si>
+    <t>It handles a 5-bus PJM network</t>
+  </si>
+  <si>
+    <t>300 MW</t>
+  </si>
+  <si>
+    <t>This paper formulates a workflow such that two models are solved. The first model represents the computation of energy price within a one-day-ahead market through two-stage stochastic program. The second model aims to minimize the charging cost while satisfying the minimum SoC.</t>
+  </si>
+  <si>
+    <t>Although the network topology is considered for experimentation, the modelling does not exploid its properties. Besides, although it takes into account the arrival and departure of vehicles, the fact of driving from an origin and destination pair is not studied.</t>
   </si>
 </sst>
 </file>
@@ -4919,7 +5031,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4978,7 +5090,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -5049,7 +5161,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6439,7 +6551,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CCC84C4-D214-284B-90BC-6A2481F38F31}">
   <dimension ref="A1:Q127"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="139" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="139" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -6471,7 +6585,7 @@
         <v>415</v>
       </c>
       <c r="E1" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="F1" t="s">
         <v>327</v>
@@ -6515,13 +6629,13 @@
         <v>844</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H2" t="s">
         <v>417</v>
@@ -6563,10 +6677,10 @@
         <v>845</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H3" t="s">
         <v>420</v>
@@ -6599,19 +6713,19 @@
         <v>44917</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>845</v>
       </c>
       <c r="E4" s="7" t="s">
+        <v>890</v>
+      </c>
+      <c r="F4" s="7" t="s">
         <v>891</v>
       </c>
-      <c r="F4" s="7" t="s">
-        <v>892</v>
-      </c>
       <c r="G4" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H4" t="s">
         <v>422</v>
@@ -6644,19 +6758,19 @@
         <v>44917</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H5" t="s">
         <v>425</v>
@@ -6689,7 +6803,7 @@
         <v>44917</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>844</v>
@@ -6731,19 +6845,19 @@
         <v>44917</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>845</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H7" t="s">
         <v>432</v>
@@ -6776,7 +6890,7 @@
         <v>44918</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>844</v>
@@ -6785,10 +6899,10 @@
         <v>845</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H8" t="s">
         <v>434</v>
@@ -6827,10 +6941,10 @@
         <v>845</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H9" t="s">
         <v>436</v>
@@ -6872,10 +6986,10 @@
         <v>845</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H10" t="s">
         <v>333</v>
@@ -6917,10 +7031,10 @@
         <v>845</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H11" t="s">
         <v>438</v>
@@ -6962,10 +7076,10 @@
         <v>845</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H12" t="s">
         <v>442</v>
@@ -6998,19 +7112,19 @@
         <v>44918</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>845</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H13" t="s">
         <v>337</v>
@@ -7043,19 +7157,19 @@
         <v>44918</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>845</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H14" t="s">
         <v>444</v>
@@ -7088,19 +7202,19 @@
         <v>44918</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>845</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H15" t="s">
         <v>448</v>
@@ -7139,13 +7253,13 @@
         <v>845</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H16" t="s">
         <v>451</v>
@@ -7187,10 +7301,10 @@
         <v>845</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H17" t="s">
         <v>454</v>
@@ -7232,10 +7346,10 @@
         <v>845</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="G18" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H18" t="s">
         <v>456</v>
@@ -7264,9 +7378,11 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B19" s="7"/>
+      <c r="B19" s="7">
+        <v>44921</v>
+      </c>
       <c r="C19" s="7" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>844</v>
@@ -7275,7 +7391,7 @@
         <v>845</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>245</v>
+        <v>331</v>
       </c>
       <c r="H19" t="s">
         <v>340</v>
@@ -7304,9 +7420,11 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B20" s="7"/>
+      <c r="B20" s="7">
+        <v>44921</v>
+      </c>
       <c r="C20" s="7" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>844</v>
@@ -7315,7 +7433,7 @@
         <v>845</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>245</v>
+        <v>329</v>
       </c>
       <c r="H20" t="s">
         <v>458</v>
@@ -7348,7 +7466,7 @@
         <v>44918</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>845</v>
@@ -7357,10 +7475,10 @@
         <v>845</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H21" t="s">
         <v>343</v>
@@ -7393,19 +7511,19 @@
         <v>44918</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>845</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H22" t="s">
         <v>348</v>
@@ -7438,19 +7556,19 @@
         <v>44918</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>845</v>
       </c>
       <c r="E23" s="7" t="s">
+        <v>919</v>
+      </c>
+      <c r="F23" s="7" t="s">
         <v>920</v>
       </c>
-      <c r="F23" s="7" t="s">
-        <v>921</v>
-      </c>
       <c r="G23" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H23" t="s">
         <v>345</v>
@@ -7483,7 +7601,7 @@
         <v>44918</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>845</v>
@@ -7492,10 +7610,10 @@
         <v>845</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H24" t="s">
         <v>464</v>
@@ -7525,10 +7643,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="7">
-        <v>44918</v>
+        <v>44921</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>844</v>
@@ -7536,8 +7654,11 @@
       <c r="E25" s="7" t="s">
         <v>845</v>
       </c>
+      <c r="F25" s="7" t="s">
+        <v>976</v>
+      </c>
       <c r="G25" s="7" t="s">
-        <v>245</v>
+        <v>867</v>
       </c>
       <c r="H25" t="s">
         <v>466</v>
@@ -7579,10 +7700,10 @@
         <v>845</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H26" t="s">
         <v>469</v>
@@ -7611,9 +7732,11 @@
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="B27" s="7"/>
+      <c r="B27" s="7">
+        <v>44921</v>
+      </c>
       <c r="C27" s="7" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D27" s="7" t="s">
         <v>844</v>
@@ -7621,8 +7744,11 @@
       <c r="E27" s="7" t="s">
         <v>845</v>
       </c>
+      <c r="F27" s="7" t="s">
+        <v>977</v>
+      </c>
       <c r="G27" s="7" t="s">
-        <v>245</v>
+        <v>867</v>
       </c>
       <c r="H27" t="s">
         <v>350</v>
@@ -7651,8 +7777,11 @@
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
+      <c r="B28" s="7">
+        <v>44921</v>
+      </c>
       <c r="C28" s="7" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="D28" s="7" t="s">
         <v>844</v>
@@ -7661,7 +7790,7 @@
         <v>845</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>245</v>
+        <v>329</v>
       </c>
       <c r="H28" t="s">
         <v>471</v>
@@ -7694,19 +7823,19 @@
         <v>44918</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D29" s="7" t="s">
         <v>845</v>
       </c>
       <c r="E29" s="7" t="s">
+        <v>890</v>
+      </c>
+      <c r="F29" s="7" t="s">
         <v>891</v>
       </c>
-      <c r="F29" s="7" t="s">
-        <v>892</v>
-      </c>
       <c r="G29" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H29" t="s">
         <v>473</v>
@@ -7745,13 +7874,13 @@
         <v>845</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="F30" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H30" t="s">
         <v>475</v>
@@ -7790,13 +7919,13 @@
         <v>845</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="F31" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H31" t="s">
         <v>478</v>
@@ -7835,13 +7964,13 @@
         <v>845</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H32" t="s">
         <v>480</v>
@@ -7883,10 +8012,10 @@
         <v>845</v>
       </c>
       <c r="F33" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H33" t="s">
         <v>482</v>
@@ -7928,10 +8057,10 @@
         <v>845</v>
       </c>
       <c r="F34" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H34" t="s">
         <v>484</v>
@@ -7970,13 +8099,13 @@
         <v>845</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="F35" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H35" t="s">
         <v>486</v>
@@ -8018,10 +8147,10 @@
         <v>845</v>
       </c>
       <c r="F36" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H36" t="s">
         <v>488</v>
@@ -8063,10 +8192,10 @@
         <v>845</v>
       </c>
       <c r="F37" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H37" t="s">
         <v>490</v>
@@ -8105,13 +8234,13 @@
         <v>845</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="F38" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H38" t="s">
         <v>492</v>
@@ -8153,10 +8282,10 @@
         <v>845</v>
       </c>
       <c r="F39" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H39" t="s">
         <v>493</v>
@@ -8189,7 +8318,7 @@
         <v>44918</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="D40" s="7" t="s">
         <v>844</v>
@@ -8198,10 +8327,10 @@
         <v>845</v>
       </c>
       <c r="F40" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H40" t="s">
         <v>353</v>
@@ -8234,19 +8363,19 @@
         <v>44916</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="D41" s="7" t="s">
         <v>845</v>
       </c>
       <c r="E41" s="7" t="s">
+        <v>890</v>
+      </c>
+      <c r="F41" t="s">
         <v>891</v>
       </c>
-      <c r="F41" t="s">
-        <v>892</v>
-      </c>
       <c r="G41" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H41" t="s">
         <v>356</v>
@@ -8277,7 +8406,7 @@
       </c>
       <c r="B42" s="7"/>
       <c r="C42" s="7" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="D42" t="s">
         <v>844</v>
@@ -8317,13 +8446,13 @@
       </c>
       <c r="B43" s="7"/>
       <c r="C43" s="7" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="D43" s="7" t="s">
         <v>844</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="G43" s="7" t="s">
         <v>245</v>
@@ -8359,7 +8488,7 @@
         <v>44921</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="D44" s="7" t="s">
         <v>845</v>
@@ -8368,10 +8497,10 @@
         <v>845</v>
       </c>
       <c r="F44" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H44" t="s">
         <v>497</v>
@@ -8402,7 +8531,7 @@
       </c>
       <c r="B45" s="7"/>
       <c r="C45" s="7" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="D45" s="7" t="s">
         <v>844</v>
@@ -8442,7 +8571,7 @@
       </c>
       <c r="B46" s="7"/>
       <c r="C46" s="7" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="D46" s="7" t="s">
         <v>844</v>
@@ -8484,7 +8613,7 @@
         <v>44921</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="D47" s="7" t="s">
         <v>845</v>
@@ -8493,10 +8622,10 @@
         <v>845</v>
       </c>
       <c r="F47" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H47" t="s">
         <v>507</v>
@@ -8529,19 +8658,19 @@
         <v>44921</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="D48" s="7" t="s">
         <v>845</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="F48" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H48" t="s">
         <v>363</v>
@@ -8574,19 +8703,19 @@
         <v>44921</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="D49" s="7" t="s">
         <v>845</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H49" t="s">
         <v>513</v>
@@ -8619,19 +8748,19 @@
         <v>44921</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="D50" s="7" t="s">
         <v>845</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H50" t="s">
         <v>517</v>
@@ -8664,19 +8793,19 @@
         <v>44921</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="D51" s="7" t="s">
         <v>845</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H51" t="s">
         <v>520</v>
@@ -8713,7 +8842,7 @@
         <v>845</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="F52" s="7" t="s">
         <v>843</v>
@@ -8753,19 +8882,19 @@
         <v>44921</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="D53" s="7" t="s">
         <v>845</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="G53" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H53" t="s">
         <v>525</v>
@@ -8808,10 +8937,10 @@
         <v>845</v>
       </c>
       <c r="F54" s="7" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="G54" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H54" t="s">
         <v>527</v>
@@ -8853,7 +8982,7 @@
         <v>845</v>
       </c>
       <c r="F55" s="7" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="G55" t="s">
         <v>843</v>
@@ -8899,10 +9028,10 @@
         <v>845</v>
       </c>
       <c r="F56" s="7" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="G56" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H56" t="s">
         <v>531</v>
@@ -8942,13 +9071,13 @@
         <v>845</v>
       </c>
       <c r="E57" s="7" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="F57" s="7" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="G57" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H57" t="s">
         <v>533</v>
@@ -8991,10 +9120,10 @@
         <v>845</v>
       </c>
       <c r="F58" s="7" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="G58" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H58" t="s">
         <v>535</v>
@@ -9037,10 +9166,10 @@
         <v>845</v>
       </c>
       <c r="F59" s="7" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="G59" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H59" t="s">
         <v>537</v>
@@ -9083,7 +9212,7 @@
         <v>845</v>
       </c>
       <c r="F60" s="7" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="G60" t="s">
         <v>843</v>
@@ -9129,10 +9258,10 @@
         <v>845</v>
       </c>
       <c r="F61" s="7" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="G61" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H61" t="s">
         <v>541</v>
@@ -9175,10 +9304,10 @@
         <v>845</v>
       </c>
       <c r="F62" s="7" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="G62" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H62" t="s">
         <v>543</v>
@@ -9221,10 +9350,10 @@
         <v>845</v>
       </c>
       <c r="F63" s="7" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="G63" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H63" t="s">
         <v>545</v>
@@ -9266,10 +9395,10 @@
         <v>845</v>
       </c>
       <c r="F64" s="7" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="G64" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H64" t="s">
         <v>547</v>
@@ -9312,10 +9441,10 @@
         <v>845</v>
       </c>
       <c r="F65" s="7" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="G65" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H65" t="s">
         <v>550</v>
@@ -9358,10 +9487,10 @@
         <v>845</v>
       </c>
       <c r="F66" s="7" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="G66" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H66" t="s">
         <v>552</v>
@@ -9404,10 +9533,10 @@
         <v>845</v>
       </c>
       <c r="F67" s="7" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="G67" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H67" t="s">
         <v>554</v>
@@ -9450,7 +9579,7 @@
         <v>845</v>
       </c>
       <c r="F68" s="7" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="G68" t="s">
         <v>843</v>
@@ -9496,10 +9625,10 @@
         <v>845</v>
       </c>
       <c r="F69" s="7" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="G69" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H69" t="s">
         <v>560</v>
@@ -9533,19 +9662,19 @@
         <v>44921</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="D70" s="7" t="s">
         <v>845</v>
       </c>
       <c r="E70" s="7" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="F70" s="7" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="G70" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H70" t="s">
         <v>366</v>
@@ -9579,7 +9708,7 @@
         <v>44921</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="D71" s="7" t="s">
         <v>845</v>
@@ -9588,10 +9717,10 @@
         <v>845</v>
       </c>
       <c r="F71" s="7" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="G71" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H71" t="s">
         <v>367</v>
@@ -9625,7 +9754,7 @@
         <v>44921</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="D72" s="7" t="s">
         <v>845</v>
@@ -9634,10 +9763,10 @@
         <v>845</v>
       </c>
       <c r="F72" s="7" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="G72" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H72" t="s">
         <v>370</v>
@@ -9671,7 +9800,7 @@
         <v>44916</v>
       </c>
       <c r="C73" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D73" t="s">
         <v>844</v>
@@ -9711,7 +9840,7 @@
       </c>
       <c r="B74" s="7"/>
       <c r="C74" s="7" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="D74" s="7" t="s">
         <v>844</v>
@@ -9751,7 +9880,7 @@
         <v>74</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="D75" s="7" t="s">
         <v>844</v>
@@ -9794,19 +9923,19 @@
         <v>44921</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="D76" s="7" t="s">
         <v>845</v>
       </c>
       <c r="E76" s="7" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="F76" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="G76" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H76" t="s">
         <v>566</v>
@@ -9849,10 +9978,10 @@
         <v>845</v>
       </c>
       <c r="F77" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="G77" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H77" t="s">
         <v>568</v>
@@ -9883,13 +10012,13 @@
         <v>77</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="D78" s="7" t="s">
         <v>844</v>
       </c>
       <c r="E78" s="7" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="G78" s="7" t="s">
         <v>245</v>
@@ -9934,10 +10063,10 @@
         <v>845</v>
       </c>
       <c r="F79" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="G79" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H79" t="s">
         <v>573</v>
@@ -9971,19 +10100,19 @@
         <v>44921</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="D80" s="7" t="s">
         <v>845</v>
       </c>
       <c r="E80" s="7" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="F80" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="G80" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H80" t="s">
         <v>575</v>
@@ -10021,10 +10150,10 @@
         <v>845</v>
       </c>
       <c r="E81" s="7" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="F81" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="G81" s="7" t="s">
         <v>843</v>
@@ -10070,10 +10199,10 @@
         <v>845</v>
       </c>
       <c r="F82" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="G82" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H82" t="s">
         <v>579</v>
@@ -10116,10 +10245,10 @@
         <v>845</v>
       </c>
       <c r="F83" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="G83" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H83" t="s">
         <v>581</v>
@@ -10162,7 +10291,7 @@
         <v>845</v>
       </c>
       <c r="G84" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H84" t="s">
         <v>583</v>
@@ -10204,10 +10333,10 @@
         <v>845</v>
       </c>
       <c r="F85" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="G85" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H85" t="s">
         <v>585</v>
@@ -10250,10 +10379,10 @@
         <v>845</v>
       </c>
       <c r="F86" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="G86" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H86" t="s">
         <v>587</v>
@@ -10296,10 +10425,10 @@
         <v>845</v>
       </c>
       <c r="F87" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="G87" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H87" t="s">
         <v>589</v>
@@ -10340,7 +10469,7 @@
         <v>845</v>
       </c>
       <c r="F88" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="G88" t="s">
         <v>843</v>
@@ -10386,10 +10515,10 @@
         <v>845</v>
       </c>
       <c r="F89" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="G89" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H89" t="s">
         <v>594</v>
@@ -10432,10 +10561,10 @@
         <v>845</v>
       </c>
       <c r="F90" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="G90" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H90" t="s">
         <v>596</v>
@@ -10478,10 +10607,10 @@
         <v>845</v>
       </c>
       <c r="F91" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="G91" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H91" t="s">
         <v>597</v>
@@ -10521,10 +10650,10 @@
         <v>845</v>
       </c>
       <c r="F92" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="G92" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H92" t="s">
         <v>599</v>
@@ -10567,10 +10696,10 @@
         <v>845</v>
       </c>
       <c r="F93" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="G93" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H93" t="s">
         <v>602</v>
@@ -10608,10 +10737,10 @@
         <v>845</v>
       </c>
       <c r="E94" s="7" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="F94" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="G94" t="s">
         <v>843</v>
@@ -10654,13 +10783,13 @@
         <v>844</v>
       </c>
       <c r="E95" s="7" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="F95" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="G95" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H95" t="s">
         <v>607</v>
@@ -10703,10 +10832,10 @@
         <v>845</v>
       </c>
       <c r="F96" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="G96" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H96" t="s">
         <v>402</v>
@@ -10746,13 +10875,13 @@
         <v>845</v>
       </c>
       <c r="E97" s="7" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="F97" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="G97" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H97" t="s">
         <v>407</v>
@@ -10783,7 +10912,7 @@
         <v>97</v>
       </c>
       <c r="C98" s="7" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="D98" s="7" t="s">
         <v>844</v>
@@ -10826,7 +10955,7 @@
         <v>44921</v>
       </c>
       <c r="C99" s="7" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D99" s="7" t="s">
         <v>845</v>
@@ -10835,10 +10964,10 @@
         <v>845</v>
       </c>
       <c r="F99" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="G99" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H99" t="s">
         <v>393</v>
@@ -10871,19 +11000,19 @@
         <v>44921</v>
       </c>
       <c r="C100" s="7" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="D100" s="7" t="s">
         <v>845</v>
       </c>
       <c r="E100" s="7" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="F100" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="G100" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H100" t="s">
         <v>611</v>
@@ -10917,19 +11046,19 @@
         <v>44921</v>
       </c>
       <c r="C101" s="7" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="D101" s="7" t="s">
         <v>845</v>
       </c>
       <c r="E101" s="7" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="F101" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="G101" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H101" t="s">
         <v>386</v>
@@ -10963,7 +11092,7 @@
         <v>44921</v>
       </c>
       <c r="C102" s="7" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D102" s="7" t="s">
         <v>845</v>
@@ -10972,10 +11101,10 @@
         <v>845</v>
       </c>
       <c r="F102" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="G102" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H102" t="s">
         <v>397</v>
@@ -11009,7 +11138,7 @@
         <v>44921</v>
       </c>
       <c r="C103" s="7" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="D103" s="7" t="s">
         <v>844</v>
@@ -11018,10 +11147,10 @@
         <v>845</v>
       </c>
       <c r="F103" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="G103" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H103" t="s">
         <v>617</v>
@@ -11055,19 +11184,19 @@
         <v>44921</v>
       </c>
       <c r="C104" s="7" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="D104" s="7" t="s">
         <v>845</v>
       </c>
       <c r="E104" s="7" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="F104" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="G104" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H104" t="s">
         <v>389</v>
@@ -11100,7 +11229,7 @@
         <v>44921</v>
       </c>
       <c r="C105" s="7" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D105" s="7" t="s">
         <v>845</v>
@@ -11109,10 +11238,10 @@
         <v>845</v>
       </c>
       <c r="F105" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="G105" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H105" t="s">
         <v>394</v>
@@ -11146,19 +11275,19 @@
         <v>44921</v>
       </c>
       <c r="C106" s="7" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="D106" s="7" t="s">
         <v>845</v>
       </c>
       <c r="E106" s="7" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="F106" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="G106" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H106" t="s">
         <v>621</v>
@@ -11191,19 +11320,19 @@
         <v>44921</v>
       </c>
       <c r="C107" s="7" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="D107" s="7" t="s">
         <v>845</v>
       </c>
       <c r="E107" s="7" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="F107" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="G107" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H107" t="s">
         <v>622</v>
@@ -11243,7 +11372,7 @@
         <v>845</v>
       </c>
       <c r="F108" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="G108" t="s">
         <v>843</v>
@@ -11283,10 +11412,10 @@
         <v>845</v>
       </c>
       <c r="E109" s="7" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="F109" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="G109" t="s">
         <v>843</v>
@@ -11329,13 +11458,13 @@
         <v>844</v>
       </c>
       <c r="E110" s="7" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="F110" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="G110" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H110" t="s">
         <v>628</v>
@@ -11375,13 +11504,13 @@
         <v>845</v>
       </c>
       <c r="E111" s="7" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="F111" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="G111" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H111" t="s">
         <v>630</v>
@@ -11421,13 +11550,13 @@
         <v>845</v>
       </c>
       <c r="E112" s="7" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="F112" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="G112" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H112" t="s">
         <v>632</v>
@@ -11470,10 +11599,10 @@
         <v>845</v>
       </c>
       <c r="F113" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="G113" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H113" t="s">
         <v>635</v>
@@ -11513,13 +11642,13 @@
         <v>844</v>
       </c>
       <c r="E114" s="7" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="F114" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="G114" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H114" t="s">
         <v>639</v>
@@ -11562,10 +11691,10 @@
         <v>845</v>
       </c>
       <c r="F115" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="G115" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H115" t="s">
         <v>641</v>
@@ -11608,10 +11737,10 @@
         <v>845</v>
       </c>
       <c r="F116" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="G116" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H116" t="s">
         <v>643</v>
@@ -11654,10 +11783,10 @@
         <v>845</v>
       </c>
       <c r="F117" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="G117" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H117" t="s">
         <v>645</v>
@@ -11696,13 +11825,13 @@
         <v>845</v>
       </c>
       <c r="E118" s="7" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="F118" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="G118" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H118" t="s">
         <v>647</v>
@@ -11744,10 +11873,10 @@
         <v>845</v>
       </c>
       <c r="F119" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="G119" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H119" t="s">
         <v>649</v>
@@ -11789,10 +11918,10 @@
         <v>845</v>
       </c>
       <c r="F120" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="G120" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H120" t="s">
         <v>651</v>
@@ -11835,10 +11964,10 @@
         <v>845</v>
       </c>
       <c r="F121" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="G121" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H121" t="s">
         <v>653</v>
@@ -11880,10 +12009,10 @@
         <v>845</v>
       </c>
       <c r="F122" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G122" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H122" t="s">
         <v>655</v>
@@ -11922,13 +12051,13 @@
         <v>845</v>
       </c>
       <c r="E123" s="7" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="F123" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="G123" s="7" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H123" t="s">
         <v>657</v>
@@ -11967,7 +12096,7 @@
         <v>845</v>
       </c>
       <c r="F124" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="G124" t="s">
         <v>843</v>
@@ -12006,10 +12135,10 @@
         <v>845</v>
       </c>
       <c r="E125" s="7" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="F125" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G125" t="s">
         <v>843</v>
@@ -12045,19 +12174,19 @@
         <v>44921</v>
       </c>
       <c r="C126" s="7" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="D126" s="7" t="s">
         <v>845</v>
       </c>
       <c r="E126" s="7" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="F126" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="G126" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H126" t="s">
         <v>401</v>
@@ -12088,13 +12217,13 @@
       </c>
       <c r="B127" s="7"/>
       <c r="C127" s="7" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="D127" s="7" t="s">
         <v>844</v>
       </c>
       <c r="E127" s="7" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="G127" t="s">
         <v>245</v>
@@ -12296,7 +12425,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7CB6A03-3DE7-FA4C-B993-C7C7A2F3853B}">
   <dimension ref="B1:U34"/>
   <sheetViews>
-    <sheetView zoomScale="151" workbookViewId="0"/>
+    <sheetView zoomScale="151" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -12772,7 +12903,7 @@
       <c r="D1" s="40"/>
       <c r="E1" s="41"/>
       <c r="K1" s="38" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="L1" s="38"/>
       <c r="M1" s="38"/>
@@ -12804,10 +12935,10 @@
         <v>6</v>
       </c>
       <c r="L2" s="36" t="s">
+        <v>927</v>
+      </c>
+      <c r="M2" s="36" t="s">
         <v>928</v>
-      </c>
-      <c r="M2" s="36" t="s">
-        <v>929</v>
       </c>
       <c r="N2" s="31" t="s">
         <v>250</v>
@@ -12819,7 +12950,7 @@
       </c>
       <c r="C3" s="31">
         <f>COUNTIF(ReadingList!$G$2:$G$122,C2)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" s="31">
         <f>COUNTIF(ReadingList!$G$2:$G$122,D2)</f>
@@ -12827,7 +12958,7 @@
       </c>
       <c r="E3" s="31">
         <f>COUNTIF(ReadingList!$G$2:$G$122,E2)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F3" s="31">
         <f>COUNTIF(ReadingList!G1:G122,"Abstract")</f>
@@ -12835,7 +12966,7 @@
       </c>
       <c r="G3" s="31">
         <f>COUNTIF(ReadingList!G1:G122,"Stand-by")</f>
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="H3" s="31">
         <f>COUNTIF(ReadingList!G1:G122,"Literature review")</f>
@@ -12846,7 +12977,7 @@
         <v>0</v>
       </c>
       <c r="K3" s="37" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="L3" s="36">
         <f>COUNTIFS(ReadingList!$D$2:$D$127,"No",ReadingList!$N$2:$N$127,"GoogleScholar")</f>
@@ -12896,10 +13027,10 @@
         <v>328</v>
       </c>
       <c r="H5" s="31" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="I5" s="31" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="J5" s="32"/>
       <c r="K5" s="37" t="s">
@@ -12932,15 +13063,15 @@
       </c>
       <c r="C6" s="31">
         <f>COUNTIF(ReadingList!G2:G122,C2) + COUNTIF(ReadingList!G2:G122,D2) + COUNTIF(ReadingList!G2:G122,E2) + COUNTIF(ReadingList!G1:G122,"Body")</f>
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="D6" s="6">
         <f>C6/F6</f>
-        <v>0.84615384615384615</v>
+        <v>0.88888888888888884</v>
       </c>
       <c r="E6" s="6">
         <f>IFERROR(SUM(C3:E3)/F6, 0)</f>
-        <v>1.7094017094017096E-2</v>
+        <v>4.2735042735042736E-2</v>
       </c>
       <c r="F6" s="31">
         <f>B6-F3-H3-I3</f>
@@ -12948,7 +13079,7 @@
       </c>
       <c r="G6" s="31">
         <f>E6*F6</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H6" s="31">
         <v>10</v>
@@ -13178,19 +13309,19 @@
       </c>
       <c r="D12" s="31">
         <f>COUNTIFS(ReadingList!$B$2:$B$122,"&lt;="&amp;B12, ReadingList!$B$2:$B$122,"&gt;"&amp;B11, ReadingList!$G$2:$G$122, $C$2) + COUNTIFS(ReadingList!$B$2:$B$122,"&lt;="&amp;B12, ReadingList!$B$2:$B$122,"&gt;"&amp;B11, ReadingList!$G$2:$G$122, $D$2) + COUNTIFS(ReadingList!$B$2:$B$122,"&lt;="&amp;B12, ReadingList!$B$2:$B$122,"&gt;"&amp;B11, ReadingList!$G$2:$G$122, $E$2) + COUNTIFS(ReadingList!$B$2:$B$122,"&lt;="&amp;B12, ReadingList!$B$2:$B$122,"&gt;"&amp;B11, ReadingList!$G$2:$G$122, "Body")</f>
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="E12" s="31">
         <f>COUNTIFS(ReadingList!$B$2:$B$122,"&lt;="&amp;B12, ReadingList!$B$2:$B$122,"&gt;"&amp;B11,ReadingList!$G$2:$G$122,$C$2) + COUNTIFS(ReadingList!$B$2:$B$122,"&lt;="&amp;B12, ReadingList!$B$2:$B$122,"&gt;"&amp;B11,ReadingList!$G$2:$G$122,$D$2) + COUNTIFS(ReadingList!$B$2:$B$122,"&lt;="&amp;B12, ReadingList!$B$2:$B$122,"&gt;"&amp;B11,ReadingList!$G$2:$G$122,$E$2)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F12" s="14">
         <f t="shared" si="0"/>
-        <v>0.48412698412698413</v>
+        <v>0.52380952380952384</v>
       </c>
       <c r="G12" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4.5454545454545456E-2</v>
       </c>
       <c r="H12" s="31" t="str">
         <f>IF(SUM($D$9:D12)&gt;=$F$6,"Finished",IF(SUM($D$9:D12)&gt;=$H$6*COUNT($B$9:B12), "Yes", "No"))</f>
@@ -13452,7 +13583,7 @@
       </c>
       <c r="H18" s="31" t="str">
         <f>IF(SUM($D$9:D18)&gt;=$F$6,"Finished",IF(SUM($D$9:D18)&gt;=$H$6*COUNT($B$9:B18), "Yes", "No"))</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="I18" s="32"/>
       <c r="J18" s="32"/>
@@ -14035,7 +14166,7 @@
       <c r="F2" s="20"/>
       <c r="G2" s="19"/>
       <c r="H2" s="44" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="I2" s="44"/>
       <c r="J2" s="44"/>
@@ -14051,7 +14182,7 @@
       <c r="F3" s="20"/>
       <c r="G3" s="19"/>
       <c r="H3" s="21" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="I3" s="21" t="s">
         <v>303</v>
@@ -14060,7 +14191,7 @@
         <v>376</v>
       </c>
       <c r="K3" s="21" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="L3" s="19"/>
     </row>
@@ -14070,7 +14201,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="D4" s="23" t="s">
         <v>0</v>
@@ -14104,13 +14235,13 @@
         <v>35</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="F5" s="42" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="G5" s="42" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="H5" s="25"/>
       <c r="I5" s="25"/>
@@ -14124,7 +14255,7 @@
       <c r="C6" s="26"/>
       <c r="D6" s="26"/>
       <c r="E6" s="26" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="F6" s="43"/>
       <c r="G6" s="43"/>
@@ -14148,13 +14279,13 @@
         <v>2</v>
       </c>
       <c r="C7" s="19" t="s">
+        <v>872</v>
+      </c>
+      <c r="D7" s="19" t="s">
         <v>873</v>
       </c>
-      <c r="D7" s="19" t="s">
-        <v>874</v>
-      </c>
       <c r="E7" s="19" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="F7" s="19"/>
       <c r="G7" s="19"/>
@@ -14170,7 +14301,7 @@
       <c r="C8" s="19"/>
       <c r="D8" s="26"/>
       <c r="E8" s="26" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="F8" s="26"/>
       <c r="G8" s="26"/>
@@ -14193,13 +14324,13 @@
       <c r="B9" s="19"/>
       <c r="C9" s="19"/>
       <c r="D9" s="19" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="E9" s="19" t="s">
+        <v>874</v>
+      </c>
+      <c r="F9" s="19" t="s">
         <v>875</v>
-      </c>
-      <c r="F9" s="19" t="s">
-        <v>876</v>
       </c>
       <c r="G9" s="19"/>
       <c r="H9" s="25">
@@ -14222,10 +14353,10 @@
         <v>3</v>
       </c>
       <c r="C10" s="22" t="s">
+        <v>876</v>
+      </c>
+      <c r="D10" s="22" t="s">
         <v>877</v>
-      </c>
-      <c r="D10" s="22" t="s">
-        <v>878</v>
       </c>
       <c r="E10" s="22"/>
       <c r="F10" s="22"/>
@@ -14248,15 +14379,15 @@
       <c r="G11" s="26"/>
       <c r="H11" s="27">
         <f>SUM(H12:H14)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I11" s="27">
         <f t="shared" ref="I11:K11" si="0">SUM(I12:I14)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J11" s="27">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K11" s="27">
         <f t="shared" si="0"/>
@@ -14270,12 +14401,12 @@
         <v>4</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="D12" s="19"/>
       <c r="E12" s="19"/>
       <c r="F12" s="23" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="G12" s="23"/>
       <c r="H12" s="23">
@@ -14284,7 +14415,7 @@
       </c>
       <c r="I12" s="23">
         <f>COUNTIFS(ReadingList!$G$2:$G$127,"SingleProblem",ReadingList!$N$2:$N$127,"WoS")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12" s="23">
         <f>COUNTIFS(ReadingList!$G$2:$G$127,"SingleProblem",ReadingList!$N$2:$N$127,"Scopus")</f>
@@ -14303,7 +14434,7 @@
       <c r="D13" s="19"/>
       <c r="E13" s="19"/>
       <c r="F13" s="23" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="G13" s="23"/>
       <c r="H13" s="23">
@@ -14331,12 +14462,12 @@
       <c r="D14" s="26"/>
       <c r="E14" s="26"/>
       <c r="F14" s="26" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="G14" s="26"/>
       <c r="H14" s="23">
         <f>COUNTIFS(ReadingList!$G$2:$G$127,"NetworkProblem",ReadingList!$N$2:$N$127,"GoogleScholar")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14" s="23">
         <f>COUNTIFS(ReadingList!$G$2:$G$127,"NetworkProblem",ReadingList!$N$2:$N$127,"WoS")</f>
@@ -14344,7 +14475,7 @@
       </c>
       <c r="J14" s="23">
         <f>COUNTIFS(ReadingList!$G$2:$G$127,"NetworkProblem",ReadingList!$N$2:$N$127,"Scopus")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K14" s="23">
         <f>COUNTIFS(ReadingList!$G$2:$G$127,"NetworkProblem",ReadingList!$N$2:$N$127,"Compendex") + COUNTIFS(ReadingList!$G$2:$G$127,"NetworkProblem",ReadingList!$N$2:$N$127,"Inspec")</f>
@@ -14385,7 +14516,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88316BFF-F978-3448-AFC7-F090CA25BADE}">
   <dimension ref="A1:BB2"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:BB2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -14605,11 +14738,14 @@
     </row>
     <row r="2" spans="1:54" s="3" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="B2" s="8">
         <f>VLOOKUP($A2,ReadingList!$A:$N,2,FALSE)</f>
-        <v>44917</v>
+        <v>44921</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>844</v>
       </c>
       <c r="D2" s="15" t="str">
         <f>VLOOKUP($A2,ReadingList!$A:$N,14,FALSE)</f>
@@ -14617,28 +14753,159 @@
       </c>
       <c r="E2" s="3">
         <f>VLOOKUP($A2,ReadingList!$A:$N,11,FALSE)</f>
-        <v>2015</v>
+        <v>2019</v>
       </c>
       <c r="F2" s="3" t="str">
         <f>VLOOKUP($A2,ReadingList!$A:$N,8,FALSE)</f>
-        <v>Deploying Public Charging Stations For Electric Vehicles On Urban Road Networks</v>
+        <v>A Two-Layer Model For Dynamic Pricing Of Electricity And Optimal Charging Of Electric Vehicles Under Price Spikes</v>
       </c>
       <c r="G2" s="3" t="str">
         <f>VLOOKUP($A2,ReadingList!$A:$N,10,FALSE)</f>
-        <v>Transportation Research Part C: Emerging Technologies</v>
+        <v>Energy</v>
       </c>
       <c r="H2" s="3" t="str">
         <f>VLOOKUP($A2,ReadingList!$A:$N,9,FALSE)</f>
-        <v>F He, Y Yin, J Zhou</v>
+        <v>V Subramanian, TK Das</v>
       </c>
       <c r="I2" s="3" t="str">
         <f>VLOOKUP($A2,ReadingList!$A:$N,13,FALSE)</f>
-        <v>This paper explores how to optimally locate public charging stations for electric vehicles on a road network, considering drivers’ spontaneous adjustments and interactions of travel and recharging decisions. The proposed approach captures the interdependency of different trips conducted by the same driver by examining the complete tour of the driver. Given the limited driving range and recharging needs of battery electric vehicles, drivers of electric vehicles are assumed to simultaneously determine tour paths and recharging plans to minimize their travel and recharging time while guaranteeing not running out of charge before completing their tours. Moreover, different initial states of charge of batteries and risk-taking attitudes of drivers toward the uncertainty of energy consumption are considered. The resulting multi-class network equilibrium flow pattern is described by a mathematical program, which is solved by an iterative procedure. Based on the proposed equilibrium framework, the charging station location problem is then formulated as a bi-level mathematical program and solved by a genetic-algorithm-based procedure. Numerical examples are presented to demonstrate the models and provide insights on public charging infrastructure deployment and behaviors of electric vehicles.</v>
-      </c>
-      <c r="Y2" s="12"/>
-      <c r="AA2" s="4"/>
-      <c r="AB2" s="4"/>
-      <c r="BB2" s="5"/>
+        <v>Pilot projects in power networks conducted across continents have established the benefits of dynamic pricing by inducing increased demand response. However, a key hurdle in the growth of demand response is the lack of widespread availability of advanced metering infrastructure, which has stymied the adoption of dynamic pricing. We believe that this hurdle will be partially addressed by the growth of electric vehicles (EVs), as smart and connected EV parking lots will be a provider of demand response. We develop a two-layer optimization model that simultaneously determines dynamic pricing policy for the system operator and demand response strategies for the EV parking lots. The model minimizes the cost to consumers, while ensuring the system operator's revenue neutral status and addressing real-time price uncertainties. A variant of the 5-bus PJM network is used to demonstrate model implementation. Numerical results show that for a low to moderate price spike scenario, dynamic pricing with demand response from EVs alone can lower the daily average consumer cost of 1.42% compared to the cost of flat pricing. A cost reduction of 6.5% is achieved when price spikes are relatively high. Computational challenges of implementing our model for real networks are discussed in the concluding remarks.</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>979</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="P2" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>2</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>850</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>850</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>896</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>844</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="Y2" s="12" t="s">
+        <v>853</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>981</v>
+      </c>
+      <c r="AA2" s="4">
+        <v>1000</v>
+      </c>
+      <c r="AB2" s="4" t="s">
+        <v>855</v>
+      </c>
+      <c r="AC2" s="3" t="s">
+        <v>982</v>
+      </c>
+      <c r="AD2" s="3" t="s">
+        <v>984</v>
+      </c>
+      <c r="AE2" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="AF2" s="3" t="s">
+        <v>902</v>
+      </c>
+      <c r="AG2" s="3" t="s">
+        <v>980</v>
+      </c>
+      <c r="AH2" s="3" t="s">
+        <v>960</v>
+      </c>
+      <c r="AI2" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="AJ2" s="3" t="s">
+        <v>844</v>
+      </c>
+      <c r="AK2" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="AL2" s="3" t="s">
+        <v>858</v>
+      </c>
+      <c r="AM2" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="AN2" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="AO2" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="AP2" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="AQ2" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="AR2" s="3" t="s">
+        <v>899</v>
+      </c>
+      <c r="AS2" s="3" t="s">
+        <v>860</v>
+      </c>
+      <c r="AT2" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="AU2" s="3" t="s">
+        <v>861</v>
+      </c>
+      <c r="AV2" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="AW2" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="AX2" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="AY2" s="3" t="s">
+        <v>985</v>
+      </c>
+      <c r="AZ2" s="3" t="s">
+        <v>986</v>
+      </c>
+      <c r="BA2" s="3" t="s">
+        <v>983</v>
+      </c>
+      <c r="BB2" s="5" t="s">
+        <v>978</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14651,7 +14918,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A4DD34D-E0D9-C545-B1E5-3E3CE99D9564}">
   <dimension ref="A1:BB2"/>
   <sheetViews>
-    <sheetView zoomScale="101" workbookViewId="0"/>
+    <sheetView topLeftCell="I1" zoomScale="101" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -14866,12 +15135,168 @@
       </c>
     </row>
     <row r="2" spans="1:54" s="3" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="13"/>
-      <c r="B2" s="8"/>
-      <c r="T2" s="12"/>
-      <c r="V2" s="4"/>
-      <c r="W2" s="4"/>
-      <c r="AV2" s="5"/>
+      <c r="A2" s="13">
+        <v>18</v>
+      </c>
+      <c r="B2" s="8">
+        <v>44921</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>844</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="E2" s="3">
+        <v>2018</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>959</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>847</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="P2" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>10</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>849</v>
+      </c>
+      <c r="T2" s="12" t="s">
+        <v>849</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>896</v>
+      </c>
+      <c r="V2" s="4" t="s">
+        <v>844</v>
+      </c>
+      <c r="W2" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>853</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>854</v>
+      </c>
+      <c r="AA2" s="3">
+        <v>289</v>
+      </c>
+      <c r="AB2" s="3" t="s">
+        <v>855</v>
+      </c>
+      <c r="AC2" s="3" t="s">
+        <v>963</v>
+      </c>
+      <c r="AD2" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="AE2" s="3" t="s">
+        <v>957</v>
+      </c>
+      <c r="AF2" s="3" t="s">
+        <v>962</v>
+      </c>
+      <c r="AG2" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="AH2" s="3" t="s">
+        <v>960</v>
+      </c>
+      <c r="AI2" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="AJ2" s="3" t="s">
+        <v>844</v>
+      </c>
+      <c r="AK2" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="AL2" s="3" t="s">
+        <v>858</v>
+      </c>
+      <c r="AM2" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="AN2" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="AO2" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="AP2" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="AQ2" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="AR2" s="3" t="s">
+        <v>899</v>
+      </c>
+      <c r="AS2" s="3" t="s">
+        <v>961</v>
+      </c>
+      <c r="AT2" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="AU2" s="3" t="s">
+        <v>966</v>
+      </c>
+      <c r="AV2" s="5" t="s">
+        <v>845</v>
+      </c>
+      <c r="AW2" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="AX2" s="3" t="s">
+        <v>965</v>
+      </c>
+      <c r="AY2" s="3" t="s">
+        <v>967</v>
+      </c>
+      <c r="AZ2" s="3" t="s">
+        <v>968</v>
+      </c>
+      <c r="BA2" s="3" t="s">
+        <v>964</v>
+      </c>
+      <c r="BB2" s="3" t="s">
+        <v>958</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14884,7 +15309,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC738410-DE0A-2D4F-A8FA-57B8B72B657E}">
   <dimension ref="A1:BB2"/>
   <sheetViews>
-    <sheetView zoomScale="101" workbookViewId="0"/>
+    <sheetView zoomScale="101" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -15132,10 +15559,10 @@
         <v>669</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>271</v>
@@ -15159,13 +15586,13 @@
         <v>271</v>
       </c>
       <c r="S2" s="3" t="s">
+        <v>895</v>
+      </c>
+      <c r="T2" s="12" t="s">
+        <v>850</v>
+      </c>
+      <c r="U2" s="3" t="s">
         <v>896</v>
-      </c>
-      <c r="T2" s="12" t="s">
-        <v>851</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>897</v>
       </c>
       <c r="V2" s="4" t="s">
         <v>845</v>
@@ -15177,19 +15604,19 @@
         <v>845</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="AA2" s="3">
         <v>2000</v>
       </c>
       <c r="AB2" s="3" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="AC2" s="3" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="AD2" s="3" t="s">
         <v>845</v>
@@ -15198,13 +15625,13 @@
         <v>845</v>
       </c>
       <c r="AF2" s="3" t="s">
+        <v>902</v>
+      </c>
+      <c r="AG2" s="3" t="s">
         <v>903</v>
       </c>
-      <c r="AG2" s="3" t="s">
-        <v>904</v>
-      </c>
       <c r="AH2" s="3" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="AI2" s="3" t="s">
         <v>207</v>
@@ -15216,10 +15643,10 @@
         <v>845</v>
       </c>
       <c r="AL2" s="3" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="AM2" s="3" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="AN2" s="3" t="s">
         <v>271</v>
@@ -15234,10 +15661,10 @@
         <v>271</v>
       </c>
       <c r="AR2" s="3" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="AS2" s="3" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="AT2" s="3" t="s">
         <v>845</v>
@@ -15249,22 +15676,22 @@
         <v>845</v>
       </c>
       <c r="AW2" s="3" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="AX2" s="3" t="s">
         <v>845</v>
       </c>
       <c r="AY2" s="3" t="s">
+        <v>906</v>
+      </c>
+      <c r="AZ2" s="3" t="s">
         <v>907</v>
       </c>
-      <c r="AZ2" s="3" t="s">
-        <v>908</v>
-      </c>
       <c r="BA2" s="3" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="BB2" s="3" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
   </sheetData>
@@ -15498,105 +15925,105 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:54" s="3" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:54" ht="323" x14ac:dyDescent="0.2">
       <c r="A2" s="13">
-        <v>73</v>
+        <v>19</v>
       </c>
       <c r="B2" s="8">
-        <v>44916</v>
+        <v>44921</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>303</v>
+        <v>376</v>
       </c>
       <c r="E2" s="3">
-        <v>2021</v>
+        <v>2018</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>562</v>
+        <v>458</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>563</v>
+        <v>459</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>565</v>
+        <v>461</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>846</v>
+        <v>969</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>135</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>848</v>
+        <v>903</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>849</v>
+        <v>139</v>
       </c>
       <c r="O2" s="3">
         <v>1</v>
       </c>
       <c r="P2" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Q2" s="3">
-        <v>3000</v>
+        <v>2</v>
       </c>
       <c r="R2" s="3" t="s">
         <v>850</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>852</v>
+        <v>896</v>
       </c>
       <c r="V2" s="3" t="s">
         <v>845</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>233</v>
+        <v>973</v>
       </c>
       <c r="X2" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="Y2" s="12" t="s">
         <v>853</v>
       </c>
-      <c r="Y2" s="12" t="s">
+      <c r="Z2" s="3" t="s">
+        <v>972</v>
+      </c>
+      <c r="AA2" s="4">
+        <v>2</v>
+      </c>
+      <c r="AB2" s="4" t="s">
+        <v>855</v>
+      </c>
+      <c r="AC2" s="3" t="s">
         <v>854</v>
       </c>
-      <c r="Z2" s="3" t="s">
-        <v>855</v>
-      </c>
-      <c r="AA2" s="4">
-        <v>3000</v>
-      </c>
-      <c r="AB2" s="4" t="s">
-        <v>856</v>
-      </c>
-      <c r="AC2" s="3" t="s">
-        <v>855</v>
-      </c>
       <c r="AD2" s="3" t="s">
-        <v>857</v>
+        <v>845</v>
       </c>
       <c r="AE2" s="3" t="s">
         <v>845</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>858</v>
+        <v>962</v>
       </c>
       <c r="AG2" s="3" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="AH2" s="3" t="s">
         <v>845</v>
@@ -15605,174 +16032,390 @@
         <v>207</v>
       </c>
       <c r="AJ2" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="AK2" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="AL2" s="3" t="s">
+        <v>858</v>
+      </c>
+      <c r="AM2" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="AN2" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="AO2" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="AP2" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="AQ2" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="AR2" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="AS2" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="AT2" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="AU2" s="3" t="s">
+        <v>966</v>
+      </c>
+      <c r="AV2" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="AW2" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="AX2" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="AY2" s="3" t="s">
+        <v>974</v>
+      </c>
+      <c r="AZ2" s="3" t="s">
+        <v>975</v>
+      </c>
+      <c r="BA2" s="3" t="s">
+        <v>970</v>
+      </c>
+      <c r="BB2" s="5" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="3" spans="1:54" ht="238" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>27</v>
+      </c>
+      <c r="B3" s="8">
+        <v>44921</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>844</v>
       </c>
-      <c r="AK2" s="3" t="s">
-        <v>845</v>
-      </c>
-      <c r="AL2" s="3" t="s">
+      <c r="D3" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="E3" s="3">
+        <v>2019</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>471</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>472</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>695</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>979</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="P3" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>2</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>850</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>850</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>896</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>844</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="Y3" s="3" t="s">
+        <v>853</v>
+      </c>
+      <c r="Z3" s="3" t="s">
+        <v>981</v>
+      </c>
+      <c r="AA3" s="3">
+        <v>1000</v>
+      </c>
+      <c r="AB3" s="3" t="s">
+        <v>855</v>
+      </c>
+      <c r="AC3" s="3" t="s">
+        <v>982</v>
+      </c>
+      <c r="AD3" s="3" t="s">
+        <v>984</v>
+      </c>
+      <c r="AE3" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="AF3" s="3" t="s">
+        <v>902</v>
+      </c>
+      <c r="AG3" s="3" t="s">
+        <v>980</v>
+      </c>
+      <c r="AH3" s="3" t="s">
+        <v>960</v>
+      </c>
+      <c r="AI3" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="AJ3" s="3" t="s">
+        <v>844</v>
+      </c>
+      <c r="AK3" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="AL3" s="3" t="s">
+        <v>858</v>
+      </c>
+      <c r="AM3" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="AN3" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="AO3" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="AP3" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="AQ3" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="AR3" s="3" t="s">
+        <v>899</v>
+      </c>
+      <c r="AS3" s="3" t="s">
+        <v>860</v>
+      </c>
+      <c r="AT3" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="AU3" s="3" t="s">
+        <v>861</v>
+      </c>
+      <c r="AV3" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="AW3" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="AX3" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="AY3" s="3" t="s">
+        <v>985</v>
+      </c>
+      <c r="AZ3" s="3" t="s">
+        <v>986</v>
+      </c>
+      <c r="BA3" s="3" t="s">
+        <v>983</v>
+      </c>
+      <c r="BB3" s="3" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="4" spans="1:54" s="3" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="13">
+        <v>73</v>
+      </c>
+      <c r="B4" s="8">
+        <v>44916</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>844</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>303</v>
+      </c>
+      <c r="E4" s="3">
+        <v>2021</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>562</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>563</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>565</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>846</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>847</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>848</v>
+      </c>
+      <c r="O4" s="3">
+        <v>1</v>
+      </c>
+      <c r="P4" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>3000</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>849</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>849</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>850</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>851</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="W4" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="X4" s="3" t="s">
+        <v>852</v>
+      </c>
+      <c r="Y4" s="12" t="s">
+        <v>853</v>
+      </c>
+      <c r="Z4" s="3" t="s">
+        <v>854</v>
+      </c>
+      <c r="AA4" s="4">
+        <v>3000</v>
+      </c>
+      <c r="AB4" s="4" t="s">
+        <v>855</v>
+      </c>
+      <c r="AC4" s="3" t="s">
+        <v>854</v>
+      </c>
+      <c r="AD4" s="3" t="s">
+        <v>856</v>
+      </c>
+      <c r="AE4" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="AF4" s="3" t="s">
+        <v>857</v>
+      </c>
+      <c r="AG4" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="AH4" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="AI4" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="AJ4" s="3" t="s">
+        <v>844</v>
+      </c>
+      <c r="AK4" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="AL4" s="3" t="s">
+        <v>858</v>
+      </c>
+      <c r="AM4" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="AN4" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="AO4" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="AP4" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="AQ4" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="AR4" s="3" t="s">
         <v>859</v>
       </c>
-      <c r="AM2" s="3" t="s">
-        <v>845</v>
-      </c>
-      <c r="AN2" s="3" t="s">
-        <v>845</v>
-      </c>
-      <c r="AO2" s="3" t="s">
-        <v>845</v>
-      </c>
-      <c r="AP2" s="3" t="s">
-        <v>845</v>
-      </c>
-      <c r="AQ2" s="3" t="s">
-        <v>845</v>
-      </c>
-      <c r="AR2" s="3" t="s">
+      <c r="AS4" s="3" t="s">
         <v>860</v>
       </c>
-      <c r="AS2" s="3" t="s">
+      <c r="AT4" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="AU4" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="AV4" s="3" t="s">
         <v>861</v>
       </c>
-      <c r="AT2" s="3" t="s">
-        <v>845</v>
-      </c>
-      <c r="AU2" s="3" t="s">
-        <v>845</v>
-      </c>
-      <c r="AV2" s="3" t="s">
+      <c r="AW4" s="3" t="s">
         <v>862</v>
       </c>
-      <c r="AW2" s="3" t="s">
+      <c r="AX4" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="AY4" s="5" t="s">
         <v>863</v>
       </c>
-      <c r="AX2" s="3" t="s">
-        <v>845</v>
-      </c>
-      <c r="AY2" s="5" t="s">
+      <c r="AZ4" s="3" t="s">
         <v>864</v>
       </c>
-      <c r="AZ2" s="3" t="s">
+      <c r="BA4" s="3" t="s">
         <v>865</v>
       </c>
-      <c r="BA2" s="3" t="s">
+      <c r="BB4" s="3" t="s">
         <v>866</v>
       </c>
-      <c r="BB2" s="3" t="s">
-        <v>867</v>
-      </c>
-    </row>
-    <row r="3" spans="1:54" x14ac:dyDescent="0.2">
-      <c r="A3" s="13"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="3"/>
-      <c r="S3" s="3"/>
-      <c r="T3" s="3"/>
-      <c r="U3" s="3"/>
-      <c r="V3" s="3"/>
-      <c r="W3" s="3"/>
-      <c r="X3" s="3"/>
-      <c r="Y3" s="12"/>
-      <c r="Z3" s="3"/>
-      <c r="AA3" s="4"/>
-      <c r="AB3" s="4"/>
-      <c r="AC3" s="3"/>
-      <c r="AD3" s="3"/>
-      <c r="AE3" s="3"/>
-      <c r="AF3" s="3"/>
-      <c r="AG3" s="3"/>
-      <c r="AH3" s="3"/>
-      <c r="AI3" s="3"/>
-      <c r="AJ3" s="3"/>
-      <c r="AK3" s="3"/>
-      <c r="AL3" s="3"/>
-      <c r="AM3" s="3"/>
-      <c r="AN3" s="3"/>
-      <c r="AO3" s="3"/>
-      <c r="AP3" s="3"/>
-      <c r="AQ3" s="3"/>
-      <c r="AR3" s="3"/>
-      <c r="AS3" s="3"/>
-      <c r="AT3" s="3"/>
-      <c r="AU3" s="3"/>
-      <c r="AV3" s="3"/>
-      <c r="AW3" s="3"/>
-      <c r="AX3" s="3"/>
-      <c r="AY3" s="3"/>
-      <c r="AZ3" s="3"/>
-      <c r="BA3" s="3"/>
-      <c r="BB3" s="5"/>
-    </row>
-    <row r="4" spans="1:54" x14ac:dyDescent="0.2">
-      <c r="A4" s="3"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
-      <c r="V4" s="3"/>
-      <c r="W4" s="3"/>
-      <c r="X4" s="3"/>
-      <c r="Y4" s="3"/>
-      <c r="Z4" s="3"/>
-      <c r="AA4" s="3"/>
-      <c r="AB4" s="3"/>
-      <c r="AC4" s="3"/>
-      <c r="AD4" s="3"/>
-      <c r="AE4" s="3"/>
-      <c r="AF4" s="3"/>
-      <c r="AG4" s="3"/>
-      <c r="AH4" s="3"/>
-      <c r="AI4" s="3"/>
-      <c r="AJ4" s="3"/>
-      <c r="AK4" s="3"/>
-      <c r="AL4" s="3"/>
-      <c r="AM4" s="3"/>
-      <c r="AN4" s="3"/>
-      <c r="AO4" s="3"/>
-      <c r="AP4" s="3"/>
-      <c r="AQ4" s="3"/>
-      <c r="AR4" s="3"/>
-      <c r="AS4" s="3"/>
-      <c r="AT4" s="3"/>
-      <c r="AU4" s="3"/>
-      <c r="AV4" s="3"/>
-      <c r="AW4" s="3"/>
-      <c r="AX4" s="3"/>
-      <c r="AY4" s="3"/>
-      <c r="AZ4" s="3"/>
-      <c r="BA4" s="3"/>
-      <c r="BB4" s="3"/>
     </row>
     <row r="5" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
@@ -16147,7 +16790,7 @@
         <v>123</v>
       </c>
       <c r="F15" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="0"/>
@@ -16276,7 +16919,7 @@
         <v>136</v>
       </c>
       <c r="F21" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="H21" t="str">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Updates the paper analysis.
</commit_message>
<xml_diff>
--- a/ReadingListAnalysis.xlsx
+++ b/ReadingListAnalysis.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
-  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usachcl-my.sharepoint.com/personal/luis_rojo_g_usach_cl/Documents/PhD/Literature_Review/Coordinated-Charging-Literature-Review/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4057" documentId="8_{11581BE0-299A-8F49-932A-90BA12D1B0CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DA67CEA2-C476-8943-BB87-41D749E69898}"/>
+  <xr:revisionPtr revIDLastSave="4363" documentId="8_{11581BE0-299A-8F49-932A-90BA12D1B0CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AFE30A3D-CE09-B445-8C55-2D71092C3510}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Dictionary!$A$1:$F$60</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ReadingList!$A$1:$N$138</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -678,7 +678,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2262" uniqueCount="987">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2371" uniqueCount="1026">
   <si>
     <t>Title</t>
   </si>
@@ -3321,9 +3321,6 @@
     <t>Selection criteria</t>
   </si>
   <si>
-    <t>Bi-level or Tri-level model</t>
-  </si>
-  <si>
     <t>Programming</t>
   </si>
   <si>
@@ -3429,9 +3426,6 @@
     <t>Not well written</t>
   </si>
   <si>
-    <t>E (completion)</t>
-  </si>
-  <si>
     <t>It is quite close to article 6 (same authors)</t>
   </si>
   <si>
@@ -3683,6 +3677,164 @@
   </si>
   <si>
     <t>Although the network topology is considered for experimentation, the modelling does not exploid its properties. Besides, although it takes into account the arrival and departure of vehicles, the fact of driving from an origin and destination pair is not studied.</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>@article{qiu2020deep,
+  title={A deep reinforcement learning method for pricing electric vehicles with discrete charging levels},
+  author={Qiu, Dawei and Ye, Yujian and Papadaskalopoulos, Dimitrios and Strbac, Goran},
+  journal={IEEE Transactions on Industry Applications},
+  volume={56},
+  number={5},
+  pages={5901--5912},
+  year={2020},
+  publisher={IEEE}
+}</t>
+  </si>
+  <si>
+    <t>Aggregators, bi-level optimization, deep learning, electricity pricing, electric vehicles (EVs)</t>
+  </si>
+  <si>
+    <t>Minimize total cost</t>
+  </si>
+  <si>
+    <t>Homogeneous (3 kW)</t>
+  </si>
+  <si>
+    <t>Hetrogeneous</t>
+  </si>
+  <si>
+    <t>UK National survey</t>
+  </si>
+  <si>
+    <t>The AU handles the charging of several home facilities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In this work, authors propose a bi-level problem identifying owners that are willing to be part of V2G charging are others that are not. To this end, the model gathers the information through a centralized approach to coordinate the charging of home facilities with different EVs. The proposed model aims to maximize the AU's profit in the upper level, and to minimize the charging cost of vehicles. It is worth noting that there is a problem for each vehicle in the lower level and therefore a constraint for each vehicle in the upper level. Then, as the often used KKT conditions does not apply given the non-convex lower problem, a deep learning-based solving method is proposed. </t>
+  </si>
+  <si>
+    <t>The novelty of the proposal is based on the solving method and the consideration of owners that are not willing to use their vehicles in the V2G charging. Despite this, the phenomena under analysis is a very particular one, and it does not consider several characteristics that are likely to change the obtained results to strengthen the insights found.</t>
+  </si>
+  <si>
+    <t>@article{zeng2020bilevel,
+  title={Bilevel robust optimization of electric vehicle charging stations with distributed energy resources},
+  author={Zeng, Bo and Dong, Houqi and Sioshansi, Ramteen and Xu, Fuqiang and Zeng, Ming},
+  journal={IEEE Transactions on Industry Applications},
+  volume={56},
+  number={5},
+  pages={5836--5847},
+  year={2020},
+  publisher={IEEE}
+}</t>
+  </si>
+  <si>
+    <t>It aims to design a public charging station</t>
+  </si>
+  <si>
+    <t>2500 kW</t>
+  </si>
+  <si>
+    <t>4 d</t>
+  </si>
+  <si>
+    <t>Bilevel optimization, charging station, distributed energy resource, energy pricing, plug-in electric vehicle (PEV), robust optimization</t>
+  </si>
+  <si>
+    <t>Sizing</t>
+  </si>
+  <si>
+    <t>Maximize utility</t>
+  </si>
+  <si>
+    <t>30 min</t>
+  </si>
+  <si>
+    <t>Many</t>
+  </si>
+  <si>
+    <t>What this study lacks is the consideration of different types of charging piles, due to a power dispatching may induce wrong insights given the power availability of extreme demand values.</t>
+  </si>
+  <si>
+    <t>This work propose a robust bi-level optimization problem to address the sizing of a single charging station considering random behavior of parameters such as arrival times, renewable energy production, among others. Besides, it considers a ToU pricing and a BESS, which may allow the CS to sell energy to the grid. Although there is no V2G, the EVs aim to maximize their utility based on a marginal price that represent the income per kWh received. On the other hand, the CSO aims to maximize its profit by planning the CS and analyzing the possible operation scenarios. Authors propose to solve the model using a single-level equivalence through KKT conditions, and a column-and-constraint generation algorithm to solve the resulting model.</t>
+  </si>
+  <si>
+    <t>Bilevel optimization problem, day-ahead market, electric vehicle, leader–follower game, regulation signal uncertainty</t>
+  </si>
+  <si>
+    <t>It handles a residential charging station</t>
+  </si>
+  <si>
+    <t>@article{cui2020optimal,
+  title={Optimal day-ahead charging and frequency reserve scheduling of electric vehicles considering the regulation signal uncertainty},
+  author={Cui, Yan and Hu, Zechun and Luo, Haocheng},
+  journal={IEEE Transactions on Industry Applications},
+  volume={56},
+  number={5},
+  pages={5824--5835},
+  year={2020},
+  publisher={IEEE}
+}</t>
+  </si>
+  <si>
+    <t>Homogeneous (7 kW)</t>
+  </si>
+  <si>
+    <t>Uniform (6 h, 8 h)</t>
+  </si>
+  <si>
+    <t>Normal (19 h, 3^2 h)</t>
+  </si>
+  <si>
+    <t>Normal (0.6, 0.1^2)</t>
+  </si>
+  <si>
+    <t>Uniform (0.9, 0.95)</t>
+  </si>
+  <si>
+    <t>PJM</t>
+  </si>
+  <si>
+    <t>20 h (12.00 - 08.00)</t>
+  </si>
+  <si>
+    <t>Authors propose a decentralized bi-level model within a day-ahead market such that pricing is used for convergence such that the AU (leader) as well as the EV owner (follower, price-taker) maximize their profits. The AU maximize their profits by setting the energy price, while prividing a virtual compensation to the EVs under a PCC for power regulation in the system. A single-level reformulation is done through a robust constraint counterpart approach, while an approximation algorithm is proposed to solve the obtained model.</t>
+  </si>
+  <si>
+    <t>Although one-day-ahead merket is under consideration, the uncertainty on arrivals and departures is not taken into account. Also, even when a decentralized control is studied, the running time of the proposed algorithm is not mentioned, and thus it might be suitable for real-time operation. Moreover, not to consider a maximum available power might produce black-outs since only system's voltage is considered. On the other hand,, a residential charging facility must consider the base-load, since infrastructure may not be able to stand the load variations.</t>
+  </si>
+  <si>
+    <t>It coordinates a bus service fleet</t>
+  </si>
+  <si>
+    <t>Electric vehicle, Real-time charging price, Demand response, Optimal charging strategy, Peak load reduction</t>
+  </si>
+  <si>
+    <t>It mentions bi-level, but it is actually two-step optimization</t>
+  </si>
+  <si>
+    <t>Agent-based modeling</t>
+  </si>
+  <si>
+    <t>Private vehicles</t>
+  </si>
+  <si>
+    <t>It has a lot of information but poorly written, it has many typos in the model</t>
+  </si>
+  <si>
+    <t>It is not in the scope given the cyber security focus</t>
+  </si>
+  <si>
+    <t>@article{li2023bi,
+  title={Bi-level programming model approach for electric vehicle charging stations considering user charging costs},
+  author={Li, Jiyong and Liu, Chengye and Wang, Yasai and Chen, Ran and Xu, Xiaoshuai},
+  journal={Electric Power Systems Research},
+  volume={214},
+  pages={108889},
+  year={2023},
+  publisher={Elsevier}
+}</t>
   </si>
 </sst>
 </file>
@@ -4270,7 +4422,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -4374,6 +4526,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="45">
@@ -5090,10 +5245,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1</c:v>
@@ -6551,11 +6706,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CCC84C4-D214-284B-90BC-6A2481F38F31}">
   <dimension ref="A1:Q127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="139" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" topLeftCell="B113" zoomScale="139" workbookViewId="0">
+      <selection activeCell="G127" sqref="G127"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
@@ -6585,7 +6740,7 @@
         <v>415</v>
       </c>
       <c r="E1" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="F1" t="s">
         <v>327</v>
@@ -6629,7 +6784,7 @@
         <v>844</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>868</v>
@@ -6713,16 +6868,16 @@
         <v>44917</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>845</v>
       </c>
       <c r="E4" s="7" t="s">
+        <v>889</v>
+      </c>
+      <c r="F4" s="7" t="s">
         <v>890</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>891</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>867</v>
@@ -6758,16 +6913,16 @@
         <v>44917</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>867</v>
@@ -6803,7 +6958,7 @@
         <v>44917</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>844</v>
@@ -6845,16 +7000,16 @@
         <v>44917</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>845</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="G7" s="7" t="s">
         <v>867</v>
@@ -6890,7 +7045,7 @@
         <v>44918</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>844</v>
@@ -6899,7 +7054,7 @@
         <v>845</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>867</v>
@@ -7076,7 +7231,7 @@
         <v>845</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="G12" s="7" t="s">
         <v>867</v>
@@ -7112,16 +7267,16 @@
         <v>44918</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>845</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="G13" s="7" t="s">
         <v>867</v>
@@ -7157,16 +7312,16 @@
         <v>44918</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>845</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="G14" s="7" t="s">
         <v>867</v>
@@ -7202,16 +7357,16 @@
         <v>44918</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>845</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="G15" s="7" t="s">
         <v>867</v>
@@ -7253,10 +7408,10 @@
         <v>845</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="G16" s="7" t="s">
         <v>867</v>
@@ -7301,7 +7456,7 @@
         <v>845</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="G17" s="7" t="s">
         <v>867</v>
@@ -7382,7 +7537,7 @@
         <v>44921</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>844</v>
@@ -7424,7 +7579,7 @@
         <v>44921</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>844</v>
@@ -7466,7 +7621,7 @@
         <v>44918</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>845</v>
@@ -7475,7 +7630,7 @@
         <v>845</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="G21" s="7" t="s">
         <v>867</v>
@@ -7511,16 +7666,16 @@
         <v>44918</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>845</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="G22" s="7" t="s">
         <v>867</v>
@@ -7556,16 +7711,16 @@
         <v>44918</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>845</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="G23" s="7" t="s">
         <v>867</v>
@@ -7601,7 +7756,7 @@
         <v>44918</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>845</v>
@@ -7610,7 +7765,7 @@
         <v>845</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="G24" s="7" t="s">
         <v>867</v>
@@ -7646,7 +7801,7 @@
         <v>44921</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>844</v>
@@ -7655,7 +7810,7 @@
         <v>845</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
       <c r="G25" s="7" t="s">
         <v>867</v>
@@ -7736,7 +7891,7 @@
         <v>44921</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="D27" s="7" t="s">
         <v>844</v>
@@ -7745,7 +7900,7 @@
         <v>845</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
       <c r="G27" s="7" t="s">
         <v>867</v>
@@ -7781,7 +7936,7 @@
         <v>44921</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D28" s="7" t="s">
         <v>844</v>
@@ -7823,16 +7978,16 @@
         <v>44918</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="D29" s="7" t="s">
         <v>845</v>
       </c>
       <c r="E29" s="7" t="s">
+        <v>889</v>
+      </c>
+      <c r="F29" s="7" t="s">
         <v>890</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>891</v>
       </c>
       <c r="G29" s="7" t="s">
         <v>867</v>
@@ -7874,10 +8029,10 @@
         <v>845</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="F30" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="G30" s="7" t="s">
         <v>867</v>
@@ -7919,10 +8074,10 @@
         <v>845</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="F31" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="G31" s="7" t="s">
         <v>867</v>
@@ -7964,10 +8119,10 @@
         <v>845</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="G32" s="7" t="s">
         <v>867</v>
@@ -8099,10 +8254,10 @@
         <v>845</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="F35" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="G35" s="7" t="s">
         <v>867</v>
@@ -8147,7 +8302,7 @@
         <v>845</v>
       </c>
       <c r="F36" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="G36" s="7" t="s">
         <v>867</v>
@@ -8234,10 +8389,10 @@
         <v>845</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="F38" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="G38" s="7" t="s">
         <v>867</v>
@@ -8282,7 +8437,7 @@
         <v>845</v>
       </c>
       <c r="F39" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="G39" s="7" t="s">
         <v>867</v>
@@ -8318,7 +8473,7 @@
         <v>44918</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D40" s="7" t="s">
         <v>844</v>
@@ -8327,7 +8482,7 @@
         <v>845</v>
       </c>
       <c r="F40" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="G40" s="7" t="s">
         <v>867</v>
@@ -8363,16 +8518,16 @@
         <v>44916</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D41" s="7" t="s">
         <v>845</v>
       </c>
       <c r="E41" s="7" t="s">
+        <v>889</v>
+      </c>
+      <c r="F41" t="s">
         <v>890</v>
-      </c>
-      <c r="F41" t="s">
-        <v>891</v>
       </c>
       <c r="G41" s="7" t="s">
         <v>867</v>
@@ -8404,9 +8559,11 @@
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="B42" s="7"/>
+      <c r="B42" s="7">
+        <v>44929</v>
+      </c>
       <c r="C42" s="7" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D42" t="s">
         <v>844</v>
@@ -8415,7 +8572,7 @@
         <v>845</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>245</v>
+        <v>332</v>
       </c>
       <c r="H42" t="s">
         <v>359</v>
@@ -8444,18 +8601,20 @@
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="B43" s="7"/>
+      <c r="B43" s="7">
+        <v>44931</v>
+      </c>
       <c r="C43" s="7" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D43" s="7" t="s">
         <v>844</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>245</v>
+        <v>331</v>
       </c>
       <c r="H43" t="s">
         <v>365</v>
@@ -8488,7 +8647,7 @@
         <v>44921</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D44" s="7" t="s">
         <v>845</v>
@@ -8497,7 +8656,7 @@
         <v>845</v>
       </c>
       <c r="F44" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="G44" s="7" t="s">
         <v>867</v>
@@ -8529,9 +8688,11 @@
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-      <c r="B45" s="7"/>
+      <c r="B45" s="7">
+        <v>44932</v>
+      </c>
       <c r="C45" s="7" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D45" s="7" t="s">
         <v>844</v>
@@ -8540,7 +8701,7 @@
         <v>845</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>245</v>
+        <v>331</v>
       </c>
       <c r="H45" t="s">
         <v>501</v>
@@ -8569,9 +8730,11 @@
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="B46" s="7"/>
+      <c r="B46" s="7">
+        <v>44932</v>
+      </c>
       <c r="C46" s="7" t="s">
-        <v>915</v>
+        <v>845</v>
       </c>
       <c r="D46" s="7" t="s">
         <v>844</v>
@@ -8580,7 +8743,7 @@
         <v>845</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>245</v>
+        <v>867</v>
       </c>
       <c r="H46" t="s">
         <v>362</v>
@@ -8613,7 +8776,7 @@
         <v>44921</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D47" s="7" t="s">
         <v>845</v>
@@ -8622,7 +8785,7 @@
         <v>845</v>
       </c>
       <c r="F47" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="G47" s="7" t="s">
         <v>867</v>
@@ -8658,16 +8821,16 @@
         <v>44921</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D48" s="7" t="s">
         <v>845</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="F48" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="G48" s="7" t="s">
         <v>867</v>
@@ -8703,16 +8866,16 @@
         <v>44921</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D49" s="7" t="s">
         <v>845</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="G49" s="7" t="s">
         <v>867</v>
@@ -8748,16 +8911,16 @@
         <v>44921</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D50" s="7" t="s">
         <v>845</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="G50" s="7" t="s">
         <v>867</v>
@@ -8793,16 +8956,16 @@
         <v>44921</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D51" s="7" t="s">
         <v>845</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="G51" s="7" t="s">
         <v>867</v>
@@ -8842,7 +9005,7 @@
         <v>845</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="F52" s="7" t="s">
         <v>843</v>
@@ -8882,16 +9045,16 @@
         <v>44921</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D53" s="7" t="s">
         <v>845</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="G53" s="7" t="s">
         <v>867</v>
@@ -8937,7 +9100,7 @@
         <v>845</v>
       </c>
       <c r="F54" s="7" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="G54" s="7" t="s">
         <v>867</v>
@@ -8982,7 +9145,7 @@
         <v>845</v>
       </c>
       <c r="F55" s="7" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="G55" t="s">
         <v>843</v>
@@ -9028,7 +9191,7 @@
         <v>845</v>
       </c>
       <c r="F56" s="7" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="G56" s="7" t="s">
         <v>867</v>
@@ -9071,10 +9234,10 @@
         <v>845</v>
       </c>
       <c r="E57" s="7" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="F57" s="7" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="G57" s="7" t="s">
         <v>867</v>
@@ -9212,7 +9375,7 @@
         <v>845</v>
       </c>
       <c r="F60" s="7" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="G60" t="s">
         <v>843</v>
@@ -9258,7 +9421,7 @@
         <v>845</v>
       </c>
       <c r="F61" s="7" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="G61" s="7" t="s">
         <v>867</v>
@@ -9304,7 +9467,7 @@
         <v>845</v>
       </c>
       <c r="F62" s="7" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
       <c r="G62" s="7" t="s">
         <v>867</v>
@@ -9350,7 +9513,7 @@
         <v>845</v>
       </c>
       <c r="F63" s="7" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="G63" s="7" t="s">
         <v>867</v>
@@ -9441,7 +9604,7 @@
         <v>845</v>
       </c>
       <c r="F65" s="7" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
       <c r="G65" s="7" t="s">
         <v>867</v>
@@ -9533,7 +9696,7 @@
         <v>845</v>
       </c>
       <c r="F67" s="7" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
       <c r="G67" s="7" t="s">
         <v>867</v>
@@ -9579,7 +9742,7 @@
         <v>845</v>
       </c>
       <c r="F68" s="7" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
       <c r="G68" t="s">
         <v>843</v>
@@ -9662,16 +9825,16 @@
         <v>44921</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D70" s="7" t="s">
         <v>845</v>
       </c>
       <c r="E70" s="7" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="F70" s="7" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="G70" s="7" t="s">
         <v>867</v>
@@ -9708,7 +9871,7 @@
         <v>44921</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D71" s="7" t="s">
         <v>845</v>
@@ -9717,7 +9880,7 @@
         <v>845</v>
       </c>
       <c r="F71" s="7" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="G71" s="7" t="s">
         <v>867</v>
@@ -9754,7 +9917,7 @@
         <v>44921</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D72" s="7" t="s">
         <v>845</v>
@@ -9763,7 +9926,7 @@
         <v>845</v>
       </c>
       <c r="F72" s="7" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="G72" s="7" t="s">
         <v>867</v>
@@ -9800,7 +9963,7 @@
         <v>44916</v>
       </c>
       <c r="C73" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="D73" t="s">
         <v>844</v>
@@ -9838,9 +10001,11 @@
         <f t="shared" si="1"/>
         <v>73</v>
       </c>
-      <c r="B74" s="7"/>
+      <c r="B74" s="7">
+        <v>44567</v>
+      </c>
       <c r="C74" s="7" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D74" s="7" t="s">
         <v>844</v>
@@ -9848,8 +10013,11 @@
       <c r="E74" s="7" t="s">
         <v>845</v>
       </c>
+      <c r="F74" s="7" t="s">
+        <v>1018</v>
+      </c>
       <c r="G74" s="7" t="s">
-        <v>245</v>
+        <v>867</v>
       </c>
       <c r="H74" t="s">
         <v>373</v>
@@ -9879,8 +10047,11 @@
         <f t="shared" si="1"/>
         <v>74</v>
       </c>
+      <c r="B75" s="7">
+        <v>44567</v>
+      </c>
       <c r="C75" s="7" t="s">
-        <v>915</v>
+        <v>845</v>
       </c>
       <c r="D75" s="7" t="s">
         <v>844</v>
@@ -9888,8 +10059,11 @@
       <c r="E75" s="7" t="s">
         <v>845</v>
       </c>
+      <c r="F75" t="s">
+        <v>1020</v>
+      </c>
       <c r="G75" s="7" t="s">
-        <v>245</v>
+        <v>867</v>
       </c>
       <c r="H75" t="s">
         <v>377</v>
@@ -9923,16 +10097,16 @@
         <v>44921</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D76" s="7" t="s">
         <v>845</v>
       </c>
       <c r="E76" s="7" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="F76" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="G76" s="7" t="s">
         <v>867</v>
@@ -10011,17 +10185,23 @@
         <f t="shared" si="1"/>
         <v>77</v>
       </c>
+      <c r="B78" s="7">
+        <v>44933</v>
+      </c>
       <c r="C78" s="7" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D78" s="7" t="s">
         <v>844</v>
       </c>
       <c r="E78" s="7" t="s">
-        <v>919</v>
+        <v>917</v>
+      </c>
+      <c r="F78" t="s">
+        <v>1023</v>
       </c>
       <c r="G78" s="7" t="s">
-        <v>245</v>
+        <v>867</v>
       </c>
       <c r="H78" t="s">
         <v>570</v>
@@ -10100,16 +10280,16 @@
         <v>44921</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D80" s="7" t="s">
         <v>845</v>
       </c>
       <c r="E80" s="7" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="F80" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="G80" s="7" t="s">
         <v>867</v>
@@ -10150,10 +10330,10 @@
         <v>845</v>
       </c>
       <c r="E81" s="7" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="F81" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
       <c r="G81" s="7" t="s">
         <v>843</v>
@@ -10379,7 +10559,7 @@
         <v>845</v>
       </c>
       <c r="F86" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="G86" s="7" t="s">
         <v>867</v>
@@ -10469,7 +10649,7 @@
         <v>845</v>
       </c>
       <c r="F88" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
       <c r="G88" t="s">
         <v>843</v>
@@ -10607,7 +10787,7 @@
         <v>845</v>
       </c>
       <c r="F91" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="G91" s="7" t="s">
         <v>867</v>
@@ -10650,7 +10830,7 @@
         <v>845</v>
       </c>
       <c r="F92" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
       <c r="G92" s="7" t="s">
         <v>867</v>
@@ -10737,10 +10917,10 @@
         <v>845</v>
       </c>
       <c r="E94" s="7" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="F94" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="G94" t="s">
         <v>843</v>
@@ -10783,7 +10963,7 @@
         <v>844</v>
       </c>
       <c r="E95" s="7" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="F95" t="s">
         <v>868</v>
@@ -10875,10 +11055,10 @@
         <v>845</v>
       </c>
       <c r="E97" s="7" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="F97" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="G97" s="7" t="s">
         <v>867</v>
@@ -10911,8 +11091,11 @@
         <f t="shared" si="1"/>
         <v>97</v>
       </c>
+      <c r="B98" s="7">
+        <v>44933</v>
+      </c>
       <c r="C98" s="7" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D98" s="7" t="s">
         <v>844</v>
@@ -10920,8 +11103,11 @@
       <c r="E98" s="7" t="s">
         <v>845</v>
       </c>
+      <c r="F98" t="s">
+        <v>1024</v>
+      </c>
       <c r="G98" s="7" t="s">
-        <v>245</v>
+        <v>867</v>
       </c>
       <c r="H98" t="s">
         <v>383</v>
@@ -10955,7 +11141,7 @@
         <v>44921</v>
       </c>
       <c r="C99" s="7" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="D99" s="7" t="s">
         <v>845</v>
@@ -10964,7 +11150,7 @@
         <v>845</v>
       </c>
       <c r="F99" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="G99" s="7" t="s">
         <v>867</v>
@@ -11000,16 +11186,16 @@
         <v>44921</v>
       </c>
       <c r="C100" s="7" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D100" s="7" t="s">
         <v>845</v>
       </c>
       <c r="E100" s="7" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="F100" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="G100" s="7" t="s">
         <v>867</v>
@@ -11046,16 +11232,16 @@
         <v>44921</v>
       </c>
       <c r="C101" s="7" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D101" s="7" t="s">
         <v>845</v>
       </c>
       <c r="E101" s="7" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="F101" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="G101" s="7" t="s">
         <v>867</v>
@@ -11092,7 +11278,7 @@
         <v>44921</v>
       </c>
       <c r="C102" s="7" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="D102" s="7" t="s">
         <v>845</v>
@@ -11101,7 +11287,7 @@
         <v>845</v>
       </c>
       <c r="F102" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="G102" s="7" t="s">
         <v>867</v>
@@ -11138,7 +11324,7 @@
         <v>44921</v>
       </c>
       <c r="C103" s="7" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D103" s="7" t="s">
         <v>844</v>
@@ -11147,7 +11333,7 @@
         <v>845</v>
       </c>
       <c r="F103" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="G103" s="7" t="s">
         <v>867</v>
@@ -11184,16 +11370,16 @@
         <v>44921</v>
       </c>
       <c r="C104" s="7" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D104" s="7" t="s">
         <v>845</v>
       </c>
       <c r="E104" s="7" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="F104" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
       <c r="G104" s="7" t="s">
         <v>867</v>
@@ -11229,7 +11415,7 @@
         <v>44921</v>
       </c>
       <c r="C105" s="7" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="D105" s="7" t="s">
         <v>845</v>
@@ -11238,7 +11424,7 @@
         <v>845</v>
       </c>
       <c r="F105" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="G105" s="7" t="s">
         <v>867</v>
@@ -11275,16 +11461,16 @@
         <v>44921</v>
       </c>
       <c r="C106" s="7" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D106" s="7" t="s">
         <v>845</v>
       </c>
       <c r="E106" s="7" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="F106" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
       <c r="G106" s="7" t="s">
         <v>867</v>
@@ -11320,16 +11506,16 @@
         <v>44921</v>
       </c>
       <c r="C107" s="7" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D107" s="7" t="s">
         <v>845</v>
       </c>
       <c r="E107" s="7" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="F107" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="G107" s="7" t="s">
         <v>867</v>
@@ -11412,10 +11598,10 @@
         <v>845</v>
       </c>
       <c r="E109" s="7" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="F109" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="G109" t="s">
         <v>843</v>
@@ -11458,10 +11644,10 @@
         <v>844</v>
       </c>
       <c r="E110" s="7" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="F110" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="G110" s="7" t="s">
         <v>867</v>
@@ -11504,10 +11690,10 @@
         <v>845</v>
       </c>
       <c r="E111" s="7" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="F111" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="G111" s="7" t="s">
         <v>867</v>
@@ -11550,10 +11736,10 @@
         <v>845</v>
       </c>
       <c r="E112" s="7" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="F112" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="G112" s="7" t="s">
         <v>867</v>
@@ -11642,7 +11828,7 @@
         <v>844</v>
       </c>
       <c r="E114" s="7" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="F114" t="s">
         <v>868</v>
@@ -11783,7 +11969,7 @@
         <v>845</v>
       </c>
       <c r="F117" t="s">
-        <v>952</v>
+        <v>950</v>
       </c>
       <c r="G117" s="7" t="s">
         <v>867</v>
@@ -11825,10 +12011,10 @@
         <v>845</v>
       </c>
       <c r="E118" s="7" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="F118" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="G118" s="7" t="s">
         <v>867</v>
@@ -12009,7 +12195,7 @@
         <v>845</v>
       </c>
       <c r="F122" t="s">
-        <v>953</v>
+        <v>951</v>
       </c>
       <c r="G122" s="7" t="s">
         <v>867</v>
@@ -12051,10 +12237,10 @@
         <v>845</v>
       </c>
       <c r="E123" s="7" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="F123" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
       <c r="G123" s="7" t="s">
         <v>867</v>
@@ -12096,7 +12282,7 @@
         <v>845</v>
       </c>
       <c r="F124" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="G124" t="s">
         <v>843</v>
@@ -12135,10 +12321,10 @@
         <v>845</v>
       </c>
       <c r="E125" s="7" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="F125" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
       <c r="G125" t="s">
         <v>843</v>
@@ -12174,16 +12360,16 @@
         <v>44921</v>
       </c>
       <c r="C126" s="7" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D126" s="7" t="s">
         <v>845</v>
       </c>
       <c r="E126" s="7" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="F126" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="G126" t="s">
         <v>867</v>
@@ -12215,18 +12401,23 @@
         <f t="shared" si="1"/>
         <v>126</v>
       </c>
-      <c r="B127" s="7"/>
+      <c r="B127" s="7">
+        <v>44933</v>
+      </c>
       <c r="C127" s="7" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D127" s="7" t="s">
         <v>844</v>
       </c>
       <c r="E127" s="7" t="s">
-        <v>931</v>
+        <v>917</v>
+      </c>
+      <c r="F127" t="s">
+        <v>974</v>
       </c>
       <c r="G127" t="s">
-        <v>245</v>
+        <v>867</v>
       </c>
       <c r="H127" t="s">
         <v>399</v>
@@ -12259,7 +12450,7 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N122">
     <sortCondition ref="K2:K122"/>
   </sortState>
-  <conditionalFormatting sqref="G89:G120 G122:G127 G7:G11 G2:G5 G14:G33 G35:G58 G60:G87">
+  <conditionalFormatting sqref="G89:G120 G122:G127 G7:G11 G2:G5 G14:G33 G60:G87 G35:G58">
     <cfRule type="containsText" dxfId="46" priority="46" stopIfTrue="1" operator="containsText" text="NetworkProblem">
       <formula>NOT(ISERROR(SEARCH("NetworkProblem",G2)))</formula>
     </cfRule>
@@ -12425,11 +12616,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7CB6A03-3DE7-FA4C-B993-C7C7A2F3853B}">
   <dimension ref="B1:U34"/>
   <sheetViews>
-    <sheetView zoomScale="151" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
-    </sheetView>
+    <sheetView zoomScale="151" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="1.6640625" style="29" customWidth="1"/>
     <col min="2" max="2" width="10.1640625" style="29" bestFit="1" customWidth="1"/>
@@ -12444,7 +12633,7 @@
     <col min="11" max="11" width="13.1640625" style="29" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.6640625" style="29" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="19.83203125" style="29" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5" style="29" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.33203125" style="29" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9.6640625" style="29" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.83203125" style="29" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="16.5" style="29" bestFit="1" customWidth="1"/>
@@ -12903,7 +13092,7 @@
       <c r="D1" s="40"/>
       <c r="E1" s="41"/>
       <c r="K1" s="38" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="L1" s="38"/>
       <c r="M1" s="38"/>
@@ -12935,13 +13124,13 @@
         <v>6</v>
       </c>
       <c r="L2" s="36" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="M2" s="36" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="N2" s="31" t="s">
-        <v>250</v>
+        <v>985</v>
       </c>
     </row>
     <row r="3" spans="2:21" ht="16" customHeight="1" x14ac:dyDescent="0.15">
@@ -12950,11 +13139,11 @@
       </c>
       <c r="C3" s="31">
         <f>COUNTIF(ReadingList!$G$2:$G$122,C2)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D3" s="31">
         <f>COUNTIF(ReadingList!$G$2:$G$122,D2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3" s="31">
         <f>COUNTIF(ReadingList!$G$2:$G$122,E2)</f>
@@ -12966,7 +13155,7 @@
       </c>
       <c r="G3" s="31">
         <f>COUNTIF(ReadingList!G1:G122,"Stand-by")</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="H3" s="31">
         <f>COUNTIF(ReadingList!G1:G122,"Literature review")</f>
@@ -12977,7 +13166,7 @@
         <v>0</v>
       </c>
       <c r="K3" s="37" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="L3" s="36">
         <f>COUNTIFS(ReadingList!$D$2:$D$127,"No",ReadingList!$N$2:$N$127,"GoogleScholar")</f>
@@ -13002,7 +13191,7 @@
       </c>
       <c r="M4" s="36">
         <f>COUNTIFS(ReadingList!$C$2:$C$127,"No",ReadingList!$N$2:$N$127,"WoS")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N4" s="31">
         <f>COUNTIFS(ReadingList!$C$2:$C$127,"No",ReadingList!$D$2:$D$127,"No",ReadingList!$N$2:$N$127,"WoS")</f>
@@ -13027,11 +13216,9 @@
         <v>328</v>
       </c>
       <c r="H5" s="31" t="s">
-        <v>912</v>
-      </c>
-      <c r="I5" s="31" t="s">
         <v>910</v>
       </c>
+      <c r="I5" s="34"/>
       <c r="J5" s="32"/>
       <c r="K5" s="37" t="s">
         <v>376</v>
@@ -13063,15 +13250,15 @@
       </c>
       <c r="C6" s="31">
         <f>COUNTIF(ReadingList!G2:G122,C2) + COUNTIF(ReadingList!G2:G122,D2) + COUNTIF(ReadingList!G2:G122,E2) + COUNTIF(ReadingList!G1:G122,"Body")</f>
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="D6" s="6">
         <f>C6/F6</f>
-        <v>0.88888888888888884</v>
+        <v>0.95726495726495731</v>
       </c>
       <c r="E6" s="6">
         <f>IFERROR(SUM(C3:E3)/F6, 0)</f>
-        <v>4.2735042735042736E-2</v>
+        <v>6.8376068376068383E-2</v>
       </c>
       <c r="F6" s="31">
         <f>B6-F3-H3-I3</f>
@@ -13079,15 +13266,12 @@
       </c>
       <c r="G6" s="31">
         <f>E6*F6</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H6" s="31">
         <v>10</v>
       </c>
-      <c r="I6" s="33">
-        <f ca="1">OFFSET(B9,ROUNDUP(F6/AVERAGEIF(D9:D33,"&gt;0"),0)-1,0)</f>
-        <v>44922</v>
-      </c>
+      <c r="I6" s="32"/>
       <c r="J6" s="32"/>
       <c r="K6" s="37" t="s">
         <v>7</v>
@@ -13098,7 +13282,7 @@
       </c>
       <c r="M6" s="36">
         <f>COUNTIFS(ReadingList!$C$2:$C$127,"No",ReadingList!$N$2:$N$127,"Compendex")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N6" s="31">
         <f>COUNTIFS(ReadingList!$C$2:$C$127,"No",ReadingList!$D$2:$D$127,"No",ReadingList!$N$2:$N$127,"Compendex")</f>
@@ -13182,7 +13366,7 @@
       </c>
       <c r="D9" s="31">
         <f>COUNTIFS(ReadingList!$B$2:$B$122,"&lt;="&amp;B9, ReadingList!$G$2:$G$122, C2) + COUNTIFS(ReadingList!$B$2:$B$122,"&lt;="&amp;B9, ReadingList!$G$2:$G$122, D2) + COUNTIFS(ReadingList!$B$2:$B$122,"&lt;="&amp;B9, ReadingList!$G$2:$G$122, E2) + COUNTIFS(ReadingList!$B$2:$B$122,"&lt;="&amp;B9, ReadingList!$G$2:$G$122, "Body")</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E9" s="31">
         <f>COUNTIFS(ReadingList!$B$2:$B$122,"&lt;="&amp;B9,ReadingList!$G$2:$G$122,C2)+COUNTIFS(ReadingList!$B$2:$B$122,"&lt;="&amp;B9,ReadingList!$G$2:$G$122,D2)+COUNTIFS(ReadingList!$B$2:$B$122,"&lt;="&amp;B9,ReadingList!$G$2:$G$122,E2)</f>
@@ -13190,11 +13374,11 @@
       </c>
       <c r="F9" s="14">
         <f>SUM(C9:D9)/$B$6</f>
-        <v>3.968253968253968E-2</v>
+        <v>5.5555555555555552E-2</v>
       </c>
       <c r="G9" s="6">
         <f>IFERROR(E9/D9, 0)</f>
-        <v>0.2</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="H9" s="31" t="s">
         <v>271</v>
@@ -13567,19 +13751,19 @@
       </c>
       <c r="D18" s="31">
         <f>COUNTIFS(ReadingList!$B$2:$B$122,"&lt;="&amp;B18, ReadingList!$B$2:$B$122,"&gt;"&amp;B17, ReadingList!$G$2:$G$122, $C$2) + COUNTIFS(ReadingList!$B$2:$B$122,"&lt;="&amp;B18, ReadingList!$B$2:$B$122,"&gt;"&amp;B17, ReadingList!$G$2:$G$122, $D$2) + COUNTIFS(ReadingList!$B$2:$B$122,"&lt;="&amp;B18, ReadingList!$B$2:$B$122,"&gt;"&amp;B17, ReadingList!$G$2:$G$122, $E$2) + COUNTIFS(ReadingList!$B$2:$B$122,"&lt;="&amp;B18, ReadingList!$B$2:$B$122,"&gt;"&amp;B17, ReadingList!$G$2:$G$122, "Body")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" s="31">
         <f>COUNTIFS(ReadingList!$B$2:$B$122,"&lt;="&amp;B18, ReadingList!$B$2:$B$122,"&gt;"&amp;B17,ReadingList!$G$2:$G$122,$C$2) + COUNTIFS(ReadingList!$B$2:$B$122,"&lt;="&amp;B18, ReadingList!$B$2:$B$122,"&gt;"&amp;B17,ReadingList!$G$2:$G$122,$D$2) + COUNTIFS(ReadingList!$B$2:$B$122,"&lt;="&amp;B18, ReadingList!$B$2:$B$122,"&gt;"&amp;B17,ReadingList!$G$2:$G$122,$E$2)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18" s="14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7.9365079365079361E-3</v>
       </c>
       <c r="G18" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H18" s="31" t="str">
         <f>IF(SUM($D$9:D18)&gt;=$F$6,"Finished",IF(SUM($D$9:D18)&gt;=$H$6*COUNT($B$9:B18), "Yes", "No"))</f>
@@ -13653,19 +13837,19 @@
       </c>
       <c r="D20" s="31">
         <f>COUNTIFS(ReadingList!$B$2:$B$122,"&lt;="&amp;B20, ReadingList!$B$2:$B$122,"&gt;"&amp;B19, ReadingList!$G$2:$G$122, $C$2) + COUNTIFS(ReadingList!$B$2:$B$122,"&lt;="&amp;B20, ReadingList!$B$2:$B$122,"&gt;"&amp;B19, ReadingList!$G$2:$G$122, $D$2) + COUNTIFS(ReadingList!$B$2:$B$122,"&lt;="&amp;B20, ReadingList!$B$2:$B$122,"&gt;"&amp;B19, ReadingList!$G$2:$G$122, $E$2) + COUNTIFS(ReadingList!$B$2:$B$122,"&lt;="&amp;B20, ReadingList!$B$2:$B$122,"&gt;"&amp;B19, ReadingList!$G$2:$G$122, "Body")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" s="31">
         <f>COUNTIFS(ReadingList!$B$2:$B$122,"&lt;="&amp;B20, ReadingList!$B$2:$B$122,"&gt;"&amp;B19,ReadingList!$G$2:$G$122,$C$2) + COUNTIFS(ReadingList!$B$2:$B$122,"&lt;="&amp;B20, ReadingList!$B$2:$B$122,"&gt;"&amp;B19,ReadingList!$G$2:$G$122,$D$2) + COUNTIFS(ReadingList!$B$2:$B$122,"&lt;="&amp;B20, ReadingList!$B$2:$B$122,"&gt;"&amp;B19,ReadingList!$G$2:$G$122,$E$2)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F20" s="14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7.9365079365079361E-3</v>
       </c>
       <c r="G20" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20" s="31" t="str">
         <f>IF(SUM($D$9:D20)&gt;=$F$6,"Finished",IF(SUM($D$9:D20)&gt;=$H$6*COUNT($B$9:B20), "Yes", "No"))</f>
@@ -13692,19 +13876,19 @@
       </c>
       <c r="D21" s="31">
         <f>COUNTIFS(ReadingList!$B$2:$B$122,"&lt;="&amp;B21, ReadingList!$B$2:$B$122,"&gt;"&amp;B20, ReadingList!$G$2:$G$122, $C$2) + COUNTIFS(ReadingList!$B$2:$B$122,"&lt;="&amp;B21, ReadingList!$B$2:$B$122,"&gt;"&amp;B20, ReadingList!$G$2:$G$122, $D$2) + COUNTIFS(ReadingList!$B$2:$B$122,"&lt;="&amp;B21, ReadingList!$B$2:$B$122,"&gt;"&amp;B20, ReadingList!$G$2:$G$122, $E$2) + COUNTIFS(ReadingList!$B$2:$B$122,"&lt;="&amp;B21, ReadingList!$B$2:$B$122,"&gt;"&amp;B20, ReadingList!$G$2:$G$122, "Body")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E21" s="31">
         <f>COUNTIFS(ReadingList!$B$2:$B$122,"&lt;="&amp;B21, ReadingList!$B$2:$B$122,"&gt;"&amp;B20,ReadingList!$G$2:$G$122,$C$2) + COUNTIFS(ReadingList!$B$2:$B$122,"&lt;="&amp;B21, ReadingList!$B$2:$B$122,"&gt;"&amp;B20,ReadingList!$G$2:$G$122,$D$2) + COUNTIFS(ReadingList!$B$2:$B$122,"&lt;="&amp;B21, ReadingList!$B$2:$B$122,"&gt;"&amp;B20,ReadingList!$G$2:$G$122,$E$2)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21" s="14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.5873015873015872E-2</v>
       </c>
       <c r="G21" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H21" s="31" t="str">
         <f>IF(SUM($D$9:D21)&gt;=$F$6,"Finished",IF(SUM($D$9:D21)&gt;=$H$6*COUNT($B$9:B21), "Yes", "No"))</f>
@@ -13727,7 +13911,7 @@
       </c>
       <c r="D22" s="31">
         <f>COUNTIFS(ReadingList!$B$2:$B$122,"&lt;="&amp;B22, ReadingList!$B$2:$B$122,"&gt;"&amp;B21, ReadingList!$G$2:$G$122, $C$2) + COUNTIFS(ReadingList!$B$2:$B$122,"&lt;="&amp;B22, ReadingList!$B$2:$B$122,"&gt;"&amp;B21, ReadingList!$G$2:$G$122, $D$2) + COUNTIFS(ReadingList!$B$2:$B$122,"&lt;="&amp;B22, ReadingList!$B$2:$B$122,"&gt;"&amp;B21, ReadingList!$G$2:$G$122, $E$2) + COUNTIFS(ReadingList!$B$2:$B$122,"&lt;="&amp;B22, ReadingList!$B$2:$B$122,"&gt;"&amp;B21, ReadingList!$G$2:$G$122, "Body")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E22" s="31">
         <f>COUNTIFS(ReadingList!$B$2:$B$122,"&lt;="&amp;B22, ReadingList!$B$2:$B$122,"&gt;"&amp;B21,ReadingList!$G$2:$G$122,$C$2) + COUNTIFS(ReadingList!$B$2:$B$122,"&lt;="&amp;B22, ReadingList!$B$2:$B$122,"&gt;"&amp;B21,ReadingList!$G$2:$G$122,$D$2) + COUNTIFS(ReadingList!$B$2:$B$122,"&lt;="&amp;B22, ReadingList!$B$2:$B$122,"&gt;"&amp;B21,ReadingList!$G$2:$G$122,$E$2)</f>
@@ -13735,7 +13919,7 @@
       </c>
       <c r="F22" s="14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.5873015873015872E-2</v>
       </c>
       <c r="G22" s="6">
         <f t="shared" si="1"/>
@@ -14130,7 +14314,7 @@
   <sheetViews>
     <sheetView zoomScale="108" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
     <col min="2" max="2" width="2.1640625" bestFit="1" customWidth="1"/>
@@ -14138,7 +14322,7 @@
     <col min="4" max="4" width="22.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -14166,7 +14350,7 @@
       <c r="F2" s="20"/>
       <c r="G2" s="19"/>
       <c r="H2" s="44" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="I2" s="44"/>
       <c r="J2" s="44"/>
@@ -14182,7 +14366,7 @@
       <c r="F3" s="20"/>
       <c r="G3" s="19"/>
       <c r="H3" s="21" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="I3" s="21" t="s">
         <v>303</v>
@@ -14191,7 +14375,7 @@
         <v>376</v>
       </c>
       <c r="K3" s="21" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="L3" s="19"/>
     </row>
@@ -14235,13 +14419,13 @@
         <v>35</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="F5" s="42" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="G5" s="42" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="H5" s="25"/>
       <c r="I5" s="25"/>
@@ -14255,7 +14439,7 @@
       <c r="C6" s="26"/>
       <c r="D6" s="26"/>
       <c r="E6" s="26" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="F6" s="43"/>
       <c r="G6" s="43"/>
@@ -14324,7 +14508,7 @@
       <c r="B9" s="19"/>
       <c r="C9" s="19"/>
       <c r="D9" s="19" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="E9" s="19" t="s">
         <v>874</v>
@@ -14355,12 +14539,16 @@
       <c r="C10" s="22" t="s">
         <v>876</v>
       </c>
-      <c r="D10" s="22" t="s">
-        <v>877</v>
-      </c>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22" t="s">
+        <v>913</v>
+      </c>
+      <c r="F10" s="46" t="s">
+        <v>1021</v>
+      </c>
+      <c r="G10" s="46" t="s">
+        <v>1022</v>
+      </c>
       <c r="H10" s="28"/>
       <c r="I10" s="28"/>
       <c r="J10" s="28"/>
@@ -14371,19 +14559,19 @@
       <c r="A11" s="19"/>
       <c r="B11" s="26"/>
       <c r="C11" s="26"/>
-      <c r="D11" s="26" t="s">
-        <v>127</v>
-      </c>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26" t="s">
+        <v>912</v>
+      </c>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
       <c r="H11" s="27">
         <f>SUM(H12:H14)</f>
         <v>2</v>
       </c>
       <c r="I11" s="27">
         <f t="shared" ref="I11:K11" si="0">SUM(I12:I14)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J11" s="27">
         <f t="shared" si="0"/>
@@ -14401,12 +14589,12 @@
         <v>4</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="D12" s="19"/>
       <c r="E12" s="19"/>
       <c r="F12" s="23" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="G12" s="23"/>
       <c r="H12" s="23">
@@ -14415,7 +14603,7 @@
       </c>
       <c r="I12" s="23">
         <f>COUNTIFS(ReadingList!$G$2:$G$127,"SingleProblem",ReadingList!$N$2:$N$127,"WoS")</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J12" s="23">
         <f>COUNTIFS(ReadingList!$G$2:$G$127,"SingleProblem",ReadingList!$N$2:$N$127,"Scopus")</f>
@@ -14434,7 +14622,7 @@
       <c r="D13" s="19"/>
       <c r="E13" s="19"/>
       <c r="F13" s="23" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="G13" s="23"/>
       <c r="H13" s="23">
@@ -14443,7 +14631,7 @@
       </c>
       <c r="I13" s="23">
         <f>COUNTIFS(ReadingList!$G$2:$G$127,"MultiProblem",ReadingList!$N$2:$N$127,"WoS")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J13" s="23">
         <f>COUNTIFS(ReadingList!$G$2:$G$127,"MultiProblem",ReadingList!$N$2:$N$127,"Scopus")</f>
@@ -14462,7 +14650,7 @@
       <c r="D14" s="26"/>
       <c r="E14" s="26"/>
       <c r="F14" s="26" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="G14" s="26"/>
       <c r="H14" s="23">
@@ -14501,11 +14689,13 @@
       <c r="L15" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
     <mergeCell ref="F5:F6"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="H2:K2"/>
     <mergeCell ref="B15:K15"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="G10:G11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -14517,12 +14707,12 @@
   <dimension ref="A1:BB2"/>
   <sheetViews>
     <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:BB2"/>
+      <selection activeCell="BC2" sqref="BC2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.83203125" style="1"/>
     <col min="3" max="3" width="8.83203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="13" style="1" bestFit="1" customWidth="1"/>
@@ -14738,173 +14928,44 @@
     </row>
     <row r="2" spans="1:54" s="3" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13">
-        <v>27</v>
+        <v>126</v>
       </c>
       <c r="B2" s="8">
         <f>VLOOKUP($A2,ReadingList!$A:$N,2,FALSE)</f>
-        <v>44921</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>844</v>
+        <v>44933</v>
       </c>
       <c r="D2" s="15" t="str">
         <f>VLOOKUP($A2,ReadingList!$A:$N,14,FALSE)</f>
-        <v>GoogleScholar</v>
+        <v>Scopus</v>
       </c>
       <c r="E2" s="3">
         <f>VLOOKUP($A2,ReadingList!$A:$N,11,FALSE)</f>
-        <v>2019</v>
+        <v>2023</v>
       </c>
       <c r="F2" s="3" t="str">
         <f>VLOOKUP($A2,ReadingList!$A:$N,8,FALSE)</f>
-        <v>A Two-Layer Model For Dynamic Pricing Of Electricity And Optimal Charging Of Electric Vehicles Under Price Spikes</v>
+        <v>Bi-Level Programming Model Approach For Electric Vehicle Charging Stations Considering User Charging Costs</v>
       </c>
       <c r="G2" s="3" t="str">
         <f>VLOOKUP($A2,ReadingList!$A:$N,10,FALSE)</f>
-        <v>Energy</v>
+        <v>Electric Power Systems Research</v>
       </c>
       <c r="H2" s="3" t="str">
         <f>VLOOKUP($A2,ReadingList!$A:$N,9,FALSE)</f>
-        <v>V Subramanian, TK Das</v>
+        <v>Li J., Liu C., Wang Y., Chen R., Xu X.</v>
       </c>
       <c r="I2" s="3" t="str">
         <f>VLOOKUP($A2,ReadingList!$A:$N,13,FALSE)</f>
-        <v>Pilot projects in power networks conducted across continents have established the benefits of dynamic pricing by inducing increased demand response. However, a key hurdle in the growth of demand response is the lack of widespread availability of advanced metering infrastructure, which has stymied the adoption of dynamic pricing. We believe that this hurdle will be partially addressed by the growth of electric vehicles (EVs), as smart and connected EV parking lots will be a provider of demand response. We develop a two-layer optimization model that simultaneously determines dynamic pricing policy for the system operator and demand response strategies for the EV parking lots. The model minimizes the cost to consumers, while ensuring the system operator's revenue neutral status and addressing real-time price uncertainties. A variant of the 5-bus PJM network is used to demonstrate model implementation. Numerical results show that for a low to moderate price spike scenario, dynamic pricing with demand response from EVs alone can lower the daily average consumer cost of 1.42% compared to the cost of flat pricing. A cost reduction of 6.5% is achieved when price spikes are relatively high. Computational challenges of implementing our model for real networks are discussed in the concluding remarks.</v>
+        <v>The rapid development of electric vehicles (EV) has placed greater demands on the planning and construction of public electric vehicle charging stations (EVCS). As EV users are highly autonomous in their charging behavior, the interests of investors and EV users are mutually affected and challenging to balance. Therefore, this paper proposes a bi-level planning model to balance the interests of investors and EV users and optimize global economic costs while improving the service satisfaction of users. The upper-level model aims to optimize the economic cost. In contrast, the lower-level model aims to optimize the service satisfaction of EV users and characterizes the charging satisfaction of EV users through the costs of charging queuing time, distance traveled, desired to charge volume, and actual charging volume, to more accurately reflect the autonomy of EV users. A combination of fast and slow charging piles is also used for planning to meet the needs of different users and improve charging stations' operational efficiency. Finally, a case study is conducted in an area of Beijing to verify that the optimization model has the advantages of low global economic cost, short charging queuing time for users, and high service satisfaction. © 2022 Elsevier B.V.</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>979</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>845</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="P2" s="3">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="3">
-        <v>2</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>850</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>850</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>896</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>844</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>845</v>
-      </c>
-      <c r="Y2" s="12" t="s">
-        <v>853</v>
-      </c>
-      <c r="Z2" s="3" t="s">
-        <v>981</v>
-      </c>
-      <c r="AA2" s="4">
-        <v>1000</v>
-      </c>
-      <c r="AB2" s="4" t="s">
-        <v>855</v>
-      </c>
-      <c r="AC2" s="3" t="s">
-        <v>982</v>
-      </c>
-      <c r="AD2" s="3" t="s">
-        <v>984</v>
-      </c>
-      <c r="AE2" s="3" t="s">
-        <v>845</v>
-      </c>
-      <c r="AF2" s="3" t="s">
-        <v>902</v>
-      </c>
-      <c r="AG2" s="3" t="s">
-        <v>980</v>
-      </c>
-      <c r="AH2" s="3" t="s">
-        <v>960</v>
-      </c>
-      <c r="AI2" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="AJ2" s="3" t="s">
-        <v>844</v>
-      </c>
-      <c r="AK2" s="3" t="s">
-        <v>845</v>
-      </c>
-      <c r="AL2" s="3" t="s">
-        <v>858</v>
-      </c>
-      <c r="AM2" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="AN2" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="AO2" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="AP2" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="AQ2" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="AR2" s="3" t="s">
-        <v>899</v>
-      </c>
-      <c r="AS2" s="3" t="s">
-        <v>860</v>
-      </c>
-      <c r="AT2" s="3" t="s">
-        <v>845</v>
-      </c>
-      <c r="AU2" s="3" t="s">
-        <v>861</v>
-      </c>
-      <c r="AV2" s="3" t="s">
-        <v>845</v>
-      </c>
-      <c r="AW2" s="3" t="s">
-        <v>845</v>
-      </c>
-      <c r="AX2" s="3" t="s">
-        <v>845</v>
-      </c>
-      <c r="AY2" s="3" t="s">
-        <v>985</v>
-      </c>
-      <c r="AZ2" s="3" t="s">
-        <v>986</v>
-      </c>
-      <c r="BA2" s="3" t="s">
-        <v>983</v>
-      </c>
+        <v>1019</v>
+      </c>
+      <c r="Y2" s="12"/>
+      <c r="AA2" s="4"/>
+      <c r="AB2" s="4"/>
       <c r="BB2" s="5" t="s">
-        <v>978</v>
+        <v>1025</v>
       </c>
     </row>
   </sheetData>
@@ -14916,11 +14977,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A4DD34D-E0D9-C545-B1E5-3E3CE99D9564}">
-  <dimension ref="A1:BB2"/>
+  <dimension ref="A1:BB4"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView zoomScale="101" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -15163,7 +15222,7 @@
         <v>342</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>845</v>
@@ -15196,7 +15255,7 @@
         <v>849</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="V2" s="4" t="s">
         <v>844</v>
@@ -15220,22 +15279,22 @@
         <v>855</v>
       </c>
       <c r="AC2" s="3" t="s">
-        <v>963</v>
+        <v>961</v>
       </c>
       <c r="AD2" s="3" t="s">
         <v>845</v>
       </c>
       <c r="AE2" s="3" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
       <c r="AG2" s="3" t="s">
         <v>139</v>
       </c>
       <c r="AH2" s="3" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
       <c r="AI2" s="3" t="s">
         <v>214</v>
@@ -15265,37 +15324,365 @@
         <v>271</v>
       </c>
       <c r="AR2" s="3" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="AS2" s="3" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="AT2" s="3" t="s">
         <v>845</v>
       </c>
       <c r="AU2" s="3" t="s">
+        <v>964</v>
+      </c>
+      <c r="AV2" s="5" t="s">
+        <v>845</v>
+      </c>
+      <c r="AW2" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="AX2" s="3" t="s">
+        <v>963</v>
+      </c>
+      <c r="AY2" s="3" t="s">
+        <v>965</v>
+      </c>
+      <c r="AZ2" s="3" t="s">
         <v>966</v>
       </c>
-      <c r="AV2" s="5" t="s">
-        <v>845</v>
-      </c>
-      <c r="AW2" s="3" t="s">
-        <v>845</v>
-      </c>
-      <c r="AX2" s="3" t="s">
-        <v>965</v>
-      </c>
-      <c r="AY2" s="3" t="s">
-        <v>967</v>
-      </c>
-      <c r="AZ2" s="3" t="s">
-        <v>968</v>
-      </c>
       <c r="BA2" s="3" t="s">
+        <v>962</v>
+      </c>
+      <c r="BB2" s="3" t="s">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="3" spans="1:54" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>42</v>
+      </c>
+      <c r="B3" s="8">
+        <v>44931</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>844</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="E3" s="3">
+        <v>2020</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>495</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>496</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>999</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>1000</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>847</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="P3" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>1003</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>849</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>1001</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>895</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="Y3" s="3" t="s">
+        <v>853</v>
+      </c>
+      <c r="Z3" s="3" t="s">
+        <v>854</v>
+      </c>
+      <c r="AA3" s="3" t="s">
+        <v>1003</v>
+      </c>
+      <c r="AB3" s="3" t="s">
+        <v>855</v>
+      </c>
+      <c r="AC3" s="3" t="s">
+        <v>854</v>
+      </c>
+      <c r="AD3" s="3" t="s">
+        <v>997</v>
+      </c>
+      <c r="AE3" s="3" t="s">
+        <v>955</v>
+      </c>
+      <c r="AF3" s="3" t="s">
+        <v>857</v>
+      </c>
+      <c r="AG3" s="3" t="s">
+        <v>847</v>
+      </c>
+      <c r="AH3" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="AI3" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="AJ3" s="3" t="s">
+        <v>844</v>
+      </c>
+      <c r="AK3" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="AL3" s="3" t="s">
+        <v>858</v>
+      </c>
+      <c r="AM3" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="AN3" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="AO3" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="AP3" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AQ3" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="AR3" s="3" t="s">
+        <v>998</v>
+      </c>
+      <c r="AS3" s="3" t="s">
+        <v>1002</v>
+      </c>
+      <c r="AT3" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="AU3" s="3" t="s">
         <v>964</v>
       </c>
-      <c r="BB2" s="3" t="s">
-        <v>958</v>
+      <c r="AV3" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="AW3" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="AX3" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="AY3" s="3" t="s">
+        <v>1005</v>
+      </c>
+      <c r="AZ3" s="3" t="s">
+        <v>1004</v>
+      </c>
+      <c r="BA3" s="3" t="s">
+        <v>996</v>
+      </c>
+      <c r="BB3" s="3" t="s">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="4" spans="1:54" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>44</v>
+      </c>
+      <c r="B4" s="8">
+        <v>44932</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="E4" s="3">
+        <v>2020</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>501</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>502</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>504</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>1006</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="P4" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>100</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>849</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>849</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>895</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="W4" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="X4" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="Y4" s="3" t="s">
+        <v>853</v>
+      </c>
+      <c r="Z4" s="3" t="s">
+        <v>854</v>
+      </c>
+      <c r="AA4" s="3">
+        <v>1000</v>
+      </c>
+      <c r="AB4" s="3" t="s">
+        <v>855</v>
+      </c>
+      <c r="AC4" s="3" t="s">
+        <v>1009</v>
+      </c>
+      <c r="AD4" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="AE4" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="AF4" s="3" t="s">
+        <v>960</v>
+      </c>
+      <c r="AG4" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="AH4" s="3" t="s">
+        <v>897</v>
+      </c>
+      <c r="AI4" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="AJ4" s="3" t="s">
+        <v>844</v>
+      </c>
+      <c r="AK4" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="AL4" s="3" t="s">
+        <v>858</v>
+      </c>
+      <c r="AM4" s="3" t="s">
+        <v>1014</v>
+      </c>
+      <c r="AN4" s="3" t="s">
+        <v>1011</v>
+      </c>
+      <c r="AO4" s="3" t="s">
+        <v>1010</v>
+      </c>
+      <c r="AP4" s="3" t="s">
+        <v>1012</v>
+      </c>
+      <c r="AQ4" s="3" t="s">
+        <v>1013</v>
+      </c>
+      <c r="AR4" s="3" t="s">
+        <v>1015</v>
+      </c>
+      <c r="AS4" s="3" t="s">
+        <v>1002</v>
+      </c>
+      <c r="AT4" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="AU4" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="AV4" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="AW4" s="3" t="s">
+        <v>861</v>
+      </c>
+      <c r="AX4" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="AY4" s="3" t="s">
+        <v>1016</v>
+      </c>
+      <c r="AZ4" s="3" t="s">
+        <v>1017</v>
+      </c>
+      <c r="BA4" s="3" t="s">
+        <v>1007</v>
+      </c>
+      <c r="BB4" s="3" t="s">
+        <v>1008</v>
       </c>
     </row>
   </sheetData>
@@ -15307,10 +15694,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC738410-DE0A-2D4F-A8FA-57B8B72B657E}">
-  <dimension ref="A1:BB2"/>
+  <dimension ref="A1:BB3"/>
   <sheetViews>
-    <sheetView zoomScale="101" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView topLeftCell="N1" zoomScale="101" workbookViewId="0">
+      <selection activeCell="AU3" sqref="AU3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15559,7 +15946,7 @@
         <v>669</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>845</v>
@@ -15586,13 +15973,13 @@
         <v>271</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="T2" s="12" t="s">
         <v>850</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="V2" s="4" t="s">
         <v>845</v>
@@ -15607,7 +15994,7 @@
         <v>853</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="AA2" s="3">
         <v>2000</v>
@@ -15616,7 +16003,7 @@
         <v>855</v>
       </c>
       <c r="AC2" s="3" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="AD2" s="3" t="s">
         <v>845</v>
@@ -15625,13 +16012,13 @@
         <v>845</v>
       </c>
       <c r="AF2" s="3" t="s">
+        <v>901</v>
+      </c>
+      <c r="AG2" s="3" t="s">
         <v>902</v>
       </c>
-      <c r="AG2" s="3" t="s">
-        <v>903</v>
-      </c>
       <c r="AH2" s="3" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="AI2" s="3" t="s">
         <v>207</v>
@@ -15646,7 +16033,7 @@
         <v>858</v>
       </c>
       <c r="AM2" s="3" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="AN2" s="3" t="s">
         <v>271</v>
@@ -15661,7 +16048,7 @@
         <v>271</v>
       </c>
       <c r="AR2" s="3" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="AS2" s="3" t="s">
         <v>860</v>
@@ -15682,16 +16069,180 @@
         <v>845</v>
       </c>
       <c r="AY2" s="3" t="s">
+        <v>905</v>
+      </c>
+      <c r="AZ2" s="3" t="s">
         <v>906</v>
       </c>
-      <c r="AZ2" s="3" t="s">
-        <v>907</v>
-      </c>
       <c r="BA2" s="3" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="BB2" s="3" t="s">
-        <v>893</v>
+        <v>892</v>
+      </c>
+    </row>
+    <row r="3" spans="1:54" s="3" customFormat="1" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>41</v>
+      </c>
+      <c r="B3" s="8">
+        <v>44929</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>844</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="E3" s="3">
+        <v>2020</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>987</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="P3" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>1000</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>849</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>988</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>895</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>844</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="Y3" s="3" t="s">
+        <v>853</v>
+      </c>
+      <c r="Z3" s="3" t="s">
+        <v>990</v>
+      </c>
+      <c r="AA3" s="3">
+        <v>1000</v>
+      </c>
+      <c r="AB3" s="3" t="s">
+        <v>855</v>
+      </c>
+      <c r="AC3" s="3" t="s">
+        <v>989</v>
+      </c>
+      <c r="AD3" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="AE3" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="AF3" s="3" t="s">
+        <v>857</v>
+      </c>
+      <c r="AG3" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="AH3" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="AI3" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="AJ3" s="3" t="s">
+        <v>844</v>
+      </c>
+      <c r="AK3" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="AL3" s="3" t="s">
+        <v>858</v>
+      </c>
+      <c r="AM3" s="3" t="s">
+        <v>991</v>
+      </c>
+      <c r="AN3" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="AO3" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="AP3" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="AQ3" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="AR3" s="3" t="s">
+        <v>898</v>
+      </c>
+      <c r="AS3" s="3" t="s">
+        <v>860</v>
+      </c>
+      <c r="AT3" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="AU3" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="AV3" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="AW3" s="3" t="s">
+        <v>862</v>
+      </c>
+      <c r="AX3" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="AY3" s="3" t="s">
+        <v>993</v>
+      </c>
+      <c r="AZ3" s="3" t="s">
+        <v>994</v>
+      </c>
+      <c r="BA3" s="3" t="s">
+        <v>992</v>
+      </c>
+      <c r="BB3" s="3" t="s">
+        <v>986</v>
       </c>
     </row>
   </sheetData>
@@ -15705,7 +16256,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD9E4D8B-4133-484F-ABD6-81FC95802664}">
   <dimension ref="A1:BB5"/>
   <sheetViews>
-    <sheetView zoomScale="101" workbookViewId="0"/>
+    <sheetView topLeftCell="A4" zoomScale="101" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -15954,7 +16507,7 @@
         <v>461</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>845</v>
@@ -15963,7 +16516,7 @@
         <v>135</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="N2" s="3" t="s">
         <v>139</v>
@@ -15987,13 +16540,13 @@
         <v>849</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="V2" s="3" t="s">
         <v>845</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
       <c r="X2" s="3" t="s">
         <v>845</v>
@@ -16002,7 +16555,7 @@
         <v>853</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
       <c r="AA2" s="4">
         <v>2</v>
@@ -16020,7 +16573,7 @@
         <v>845</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
       <c r="AG2" s="3" t="s">
         <v>139</v>
@@ -16065,7 +16618,7 @@
         <v>845</v>
       </c>
       <c r="AU2" s="3" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
       <c r="AV2" s="3" t="s">
         <v>845</v>
@@ -16077,16 +16630,16 @@
         <v>845</v>
       </c>
       <c r="AY2" s="3" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
       <c r="AZ2" s="3" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
       <c r="BA2" s="3" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
       <c r="BB2" s="5" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
     </row>
     <row r="3" spans="1:54" ht="238" x14ac:dyDescent="0.2">
@@ -16118,7 +16671,7 @@
         <v>695</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>845</v>
@@ -16151,7 +16704,7 @@
         <v>850</v>
       </c>
       <c r="U3" s="3" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="V3" s="3" t="s">
         <v>844</v>
@@ -16166,7 +16719,7 @@
         <v>853</v>
       </c>
       <c r="Z3" s="3" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
       <c r="AA3" s="3">
         <v>1000</v>
@@ -16175,22 +16728,22 @@
         <v>855</v>
       </c>
       <c r="AC3" s="3" t="s">
+        <v>980</v>
+      </c>
+      <c r="AD3" s="3" t="s">
         <v>982</v>
       </c>
-      <c r="AD3" s="3" t="s">
-        <v>984</v>
-      </c>
       <c r="AE3" s="3" t="s">
         <v>845</v>
       </c>
       <c r="AF3" s="3" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="AG3" s="3" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
       <c r="AH3" s="3" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
       <c r="AI3" s="3" t="s">
         <v>207</v>
@@ -16220,7 +16773,7 @@
         <v>271</v>
       </c>
       <c r="AR3" s="3" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="AS3" s="3" t="s">
         <v>860</v>
@@ -16241,16 +16794,16 @@
         <v>845</v>
       </c>
       <c r="AY3" s="3" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
       <c r="AZ3" s="3" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
       <c r="BA3" s="3" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
       <c r="BB3" s="3" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
     </row>
     <row r="4" spans="1:54" s="3" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
@@ -16790,7 +17343,7 @@
         <v>123</v>
       </c>
       <c r="F15" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="0"/>
@@ -16919,7 +17472,7 @@
         <v>136</v>
       </c>
       <c r="F21" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
       <c r="H21" t="str">
         <f t="shared" si="0"/>

</xml_diff>